<commit_message>
change coupling double spreadsheet
</commit_message>
<xml_diff>
--- a/coupling_phip/csv/05-19_double/csv/xlsx/Stock solution for Piperazine Imidazole .xlsx
+++ b/coupling_phip/csv/05-19_double/csv/xlsx/Stock solution for Piperazine Imidazole .xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdi35357\CODING\github_repo\OT1-coding\coupling_phip\csv\05-19_double\csv\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="13830"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Location</t>
   </si>
@@ -46,15 +54,6 @@
     <t>Volume to dispense</t>
   </si>
   <si>
-    <t>n (mmol)</t>
-  </si>
-  <si>
-    <t>Volume_stock per reaction</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>Piperazine-1</t>
   </si>
   <si>
@@ -64,46 +63,47 @@
     <t>C8H14Cl2N4O</t>
   </si>
   <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>Piperazine-2</t>
-  </si>
-  <si>
-    <t>A3</t>
   </si>
   <si>
     <t>Piperazine-3</t>
   </si>
   <si>
-    <t>A4</t>
+    <t>B1</t>
   </si>
   <si>
-    <t>Piperazine-4</t>
+    <t>B2</t>
   </si>
   <si>
-    <t>A5</t>
+    <t>B3</t>
   </si>
   <si>
-    <t>Piperazine-5</t>
+    <t>Volume max per vial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,64 +111,331 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L995"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="3" width="8.71"/>
-    <col customWidth="1" min="4" max="4" width="12.43"/>
-    <col customWidth="1" min="5" max="5" width="8.71"/>
-    <col customWidth="1" min="6" max="6" width="6.71"/>
-    <col customWidth="1" min="7" max="8" width="8.71"/>
-    <col customWidth="1" min="9" max="9" width="26.29"/>
-    <col customWidth="1" min="10" max="10" width="17.14"/>
-    <col customWidth="1" min="11" max="11" width="8.71"/>
-    <col customWidth="1" min="12" max="14" width="11.86"/>
-    <col customWidth="1" min="15" max="16" width="8.71"/>
-    <col customWidth="1" min="17" max="17" width="11.86"/>
-    <col customWidth="1" min="18" max="26" width="8.71"/>
+    <col min="1" max="3" width="8.75" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
+    <col min="6" max="6" width="6.75" customWidth="1"/>
+    <col min="7" max="8" width="8.75" customWidth="1"/>
+    <col min="9" max="9" width="13.75" customWidth="1"/>
+    <col min="10" max="10" width="5.375" customWidth="1"/>
+    <col min="11" max="11" width="8.75" customWidth="1"/>
+    <col min="12" max="12" width="11.875" customWidth="1"/>
+    <col min="13" max="14" width="8.75" customWidth="1"/>
+    <col min="15" max="15" width="11.875" customWidth="1"/>
+    <col min="16" max="24" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -202,3209 +469,3122 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="1">
         <v>253.13</v>
       </c>
       <c r="F2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" ref="G2:G6" si="1">F2/E2/1500*1000</f>
-        <v>5.267385665</v>
+        <f t="shared" ref="G2:G4" si="0">F2/E2/1500*1000</f>
+        <v>5.2673856648099129</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H6" si="2">G2/2</f>
-        <v>2.633692832</v>
+        <f t="shared" ref="H2:H4" si="1">G2/2</f>
+        <v>2.6336928324049564</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I6" si="3">G2*1000</f>
-        <v>5267.385665</v>
+        <f t="shared" ref="I2:I4" si="2">G2*1000</f>
+        <v>5267.3856648099127</v>
       </c>
       <c r="J2">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="K2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="L2">
-        <v>0.07</v>
-      </c>
-      <c r="M2">
-        <f t="shared" ref="M2:M6" si="4">ROUND(L2/J2*1000000,1)</f>
-        <v>46.7</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
+        <f>K2-100</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>253.13</v>
       </c>
       <c r="F3">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="G3" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2673856648099129</v>
+      </c>
+      <c r="H3">
         <f t="shared" si="1"/>
-        <v>5.267385665</v>
-      </c>
-      <c r="H3">
+        <v>2.6336928324049564</v>
+      </c>
+      <c r="I3">
         <f t="shared" si="2"/>
-        <v>2.633692832</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="3"/>
-        <v>5267.385665</v>
+        <v>5267.3856648099127</v>
       </c>
       <c r="J3">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="K3">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="L3">
-        <v>0.07</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="4"/>
-        <v>46.7</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
+        <f>K3-100</f>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>253.13</v>
       </c>
       <c r="F4">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2673856648099129</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="1"/>
-        <v>5.267385665</v>
-      </c>
-      <c r="H4">
+        <v>2.6336928324049564</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="2"/>
-        <v>2.633692832</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="3"/>
-        <v>5267.385665</v>
+        <v>5267.3856648099127</v>
       </c>
       <c r="J4">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="K4">
-        <v>2000.0</v>
+        <f>I4-SUM(K2:K3)</f>
+        <v>1267.3856648099127</v>
       </c>
       <c r="L4">
-        <v>0.07</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="4"/>
-        <v>46.7</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1">
-        <v>253.13</v>
-      </c>
-      <c r="F5">
-        <v>2000.0</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="1"/>
-        <v>5.267385665</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
-        <v>2.633692832</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="3"/>
-        <v>5267.385665</v>
-      </c>
-      <c r="J5">
-        <v>1500.0</v>
-      </c>
-      <c r="K5">
-        <v>2000.0</v>
-      </c>
-      <c r="L5">
-        <v>0.07</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="4"/>
-        <v>46.7</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="1">
-        <v>253.13</v>
-      </c>
-      <c r="F6">
-        <v>2000.0</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="1"/>
-        <v>5.267385665</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
-        <v>2.633692832</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="3"/>
-        <v>5267.385665</v>
-      </c>
-      <c r="J6">
-        <v>1500.0</v>
-      </c>
-      <c r="K6">
-        <v>2000.0</v>
-      </c>
-      <c r="L6">
-        <v>0.07</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="4"/>
-        <v>46.7</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
+        <f>K4-100</f>
+        <v>1167.3856648099127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" ht="14.25" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" ht="14.25" customHeight="1">
       <c r="G7" s="3"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:12" ht="14.25" customHeight="1">
       <c r="G8" s="4"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:12" ht="14.25" customHeight="1">
       <c r="G9" s="3"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:12" ht="14.25" customHeight="1">
       <c r="G10" s="3"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:12" ht="14.25" customHeight="1">
       <c r="G11" s="3"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:12" ht="14.25" customHeight="1">
       <c r="G12" s="3"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:12" ht="14.25" customHeight="1">
       <c r="G13" s="3"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:12" ht="14.25" customHeight="1">
       <c r="G14" s="3"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:12" ht="14.25" customHeight="1">
       <c r="G15" s="3"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:12" ht="14.25" customHeight="1">
       <c r="G16" s="3"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="7:7" ht="14.25" customHeight="1">
       <c r="G17" s="3"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="7:7" ht="14.25" customHeight="1">
       <c r="G18" s="3"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="7:7" ht="14.25" customHeight="1">
       <c r="G19" s="3"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="7:7" ht="14.25" customHeight="1">
       <c r="G20" s="3"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="7:7" ht="14.25" customHeight="1">
       <c r="G21" s="3"/>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="7:7" ht="14.25" customHeight="1">
       <c r="G22" s="3"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="7:7" ht="14.25" customHeight="1">
       <c r="G23" s="3"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="7:7" ht="14.25" customHeight="1">
       <c r="G24" s="3"/>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="7:7" ht="14.25" customHeight="1">
       <c r="G25" s="3"/>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="7:7" ht="14.25" customHeight="1">
       <c r="G26" s="3"/>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="7:7" ht="14.25" customHeight="1">
       <c r="G27" s="3"/>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="7:7" ht="14.25" customHeight="1">
       <c r="G28" s="3"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="7:7" ht="14.25" customHeight="1">
       <c r="G29" s="3"/>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="7:7" ht="14.25" customHeight="1">
       <c r="G30" s="3"/>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="7:7" ht="14.25" customHeight="1">
       <c r="G31" s="3"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="7:7" ht="14.25" customHeight="1">
       <c r="G32" s="3"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" spans="7:7" ht="14.25" customHeight="1">
       <c r="G33" s="3"/>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" spans="7:7" ht="14.25" customHeight="1">
       <c r="G34" s="3"/>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="7:7" ht="14.25" customHeight="1">
       <c r="G35" s="3"/>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="7:7" ht="14.25" customHeight="1">
       <c r="G36" s="3"/>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" spans="7:7" ht="14.25" customHeight="1">
       <c r="G37" s="3"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="7:7" ht="14.25" customHeight="1">
       <c r="G38" s="3"/>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="7:7" ht="14.25" customHeight="1">
       <c r="G39" s="3"/>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="7:7" ht="14.25" customHeight="1">
       <c r="G40" s="3"/>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" spans="7:7" ht="14.25" customHeight="1">
       <c r="G41" s="3"/>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" spans="7:7" ht="14.25" customHeight="1">
       <c r="G42" s="3"/>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" spans="7:7" ht="14.25" customHeight="1">
       <c r="G43" s="3"/>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
+    <row r="44" spans="7:7" ht="14.25" customHeight="1">
       <c r="G44" s="3"/>
     </row>
-    <row r="45" ht="14.25" customHeight="1">
+    <row r="45" spans="7:7" ht="14.25" customHeight="1">
       <c r="G45" s="3"/>
     </row>
-    <row r="46" ht="14.25" customHeight="1">
+    <row r="46" spans="7:7" ht="14.25" customHeight="1">
       <c r="G46" s="3"/>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
+    <row r="47" spans="7:7" ht="14.25" customHeight="1">
       <c r="G47" s="3"/>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
+    <row r="48" spans="7:7" ht="14.25" customHeight="1">
       <c r="G48" s="3"/>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
+    <row r="49" spans="7:7" ht="14.25" customHeight="1">
       <c r="G49" s="3"/>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
+    <row r="50" spans="7:7" ht="14.25" customHeight="1">
       <c r="G50" s="3"/>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" spans="7:7" ht="14.25" customHeight="1">
       <c r="G51" s="3"/>
     </row>
-    <row r="52" ht="14.25" customHeight="1">
+    <row r="52" spans="7:7" ht="14.25" customHeight="1">
       <c r="G52" s="3"/>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
+    <row r="53" spans="7:7" ht="14.25" customHeight="1">
       <c r="G53" s="3"/>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
+    <row r="54" spans="7:7" ht="14.25" customHeight="1">
       <c r="G54" s="3"/>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
+    <row r="55" spans="7:7" ht="14.25" customHeight="1">
       <c r="G55" s="3"/>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
+    <row r="56" spans="7:7" ht="14.25" customHeight="1">
       <c r="G56" s="3"/>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
+    <row r="57" spans="7:7" ht="14.25" customHeight="1">
       <c r="G57" s="3"/>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
+    <row r="58" spans="7:7" ht="14.25" customHeight="1">
       <c r="G58" s="3"/>
     </row>
-    <row r="59" ht="14.25" customHeight="1">
+    <row r="59" spans="7:7" ht="14.25" customHeight="1">
       <c r="G59" s="3"/>
     </row>
-    <row r="60" ht="14.25" customHeight="1">
+    <row r="60" spans="7:7" ht="14.25" customHeight="1">
       <c r="G60" s="3"/>
     </row>
-    <row r="61" ht="14.25" customHeight="1">
+    <row r="61" spans="7:7" ht="14.25" customHeight="1">
       <c r="G61" s="3"/>
     </row>
-    <row r="62" ht="14.25" customHeight="1">
+    <row r="62" spans="7:7" ht="14.25" customHeight="1">
       <c r="G62" s="3"/>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
+    <row r="63" spans="7:7" ht="14.25" customHeight="1">
       <c r="G63" s="3"/>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
+    <row r="64" spans="7:7" ht="14.25" customHeight="1">
       <c r="G64" s="3"/>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
+    <row r="65" spans="7:7" ht="14.25" customHeight="1">
       <c r="G65" s="3"/>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" spans="7:7" ht="14.25" customHeight="1">
       <c r="G66" s="3"/>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
+    <row r="67" spans="7:7" ht="14.25" customHeight="1">
       <c r="G67" s="3"/>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" spans="7:7" ht="14.25" customHeight="1">
       <c r="G68" s="3"/>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
+    <row r="69" spans="7:7" ht="14.25" customHeight="1">
       <c r="G69" s="3"/>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" spans="7:7" ht="14.25" customHeight="1">
       <c r="G70" s="3"/>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
+    <row r="71" spans="7:7" ht="14.25" customHeight="1">
       <c r="G71" s="3"/>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" spans="7:7" ht="14.25" customHeight="1">
       <c r="G72" s="3"/>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
+    <row r="73" spans="7:7" ht="14.25" customHeight="1">
       <c r="G73" s="3"/>
     </row>
-    <row r="74" ht="14.25" customHeight="1">
+    <row r="74" spans="7:7" ht="14.25" customHeight="1">
       <c r="G74" s="3"/>
     </row>
-    <row r="75" ht="14.25" customHeight="1">
+    <row r="75" spans="7:7" ht="14.25" customHeight="1">
       <c r="G75" s="3"/>
     </row>
-    <row r="76" ht="14.25" customHeight="1">
+    <row r="76" spans="7:7" ht="14.25" customHeight="1">
       <c r="G76" s="3"/>
     </row>
-    <row r="77" ht="14.25" customHeight="1">
+    <row r="77" spans="7:7" ht="14.25" customHeight="1">
       <c r="G77" s="3"/>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
+    <row r="78" spans="7:7" ht="14.25" customHeight="1">
       <c r="G78" s="3"/>
     </row>
-    <row r="79" ht="14.25" customHeight="1">
+    <row r="79" spans="7:7" ht="14.25" customHeight="1">
       <c r="G79" s="3"/>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
+    <row r="80" spans="7:7" ht="14.25" customHeight="1">
       <c r="G80" s="3"/>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
+    <row r="81" spans="7:7" ht="14.25" customHeight="1">
       <c r="G81" s="3"/>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
+    <row r="82" spans="7:7" ht="14.25" customHeight="1">
       <c r="G82" s="3"/>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" spans="7:7" ht="14.25" customHeight="1">
       <c r="G83" s="3"/>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
+    <row r="84" spans="7:7" ht="14.25" customHeight="1">
       <c r="G84" s="3"/>
     </row>
-    <row r="85" ht="14.25" customHeight="1">
+    <row r="85" spans="7:7" ht="14.25" customHeight="1">
       <c r="G85" s="3"/>
     </row>
-    <row r="86" ht="14.25" customHeight="1">
+    <row r="86" spans="7:7" ht="14.25" customHeight="1">
       <c r="G86" s="3"/>
     </row>
-    <row r="87" ht="14.25" customHeight="1">
+    <row r="87" spans="7:7" ht="14.25" customHeight="1">
       <c r="G87" s="3"/>
     </row>
-    <row r="88" ht="14.25" customHeight="1">
+    <row r="88" spans="7:7" ht="14.25" customHeight="1">
       <c r="G88" s="3"/>
     </row>
-    <row r="89" ht="14.25" customHeight="1">
+    <row r="89" spans="7:7" ht="14.25" customHeight="1">
       <c r="G89" s="3"/>
     </row>
-    <row r="90" ht="14.25" customHeight="1">
+    <row r="90" spans="7:7" ht="14.25" customHeight="1">
       <c r="G90" s="3"/>
     </row>
-    <row r="91" ht="14.25" customHeight="1">
+    <row r="91" spans="7:7" ht="14.25" customHeight="1">
       <c r="G91" s="3"/>
     </row>
-    <row r="92" ht="14.25" customHeight="1">
+    <row r="92" spans="7:7" ht="14.25" customHeight="1">
       <c r="G92" s="3"/>
     </row>
-    <row r="93" ht="14.25" customHeight="1">
+    <row r="93" spans="7:7" ht="14.25" customHeight="1">
       <c r="G93" s="3"/>
     </row>
-    <row r="94" ht="14.25" customHeight="1">
+    <row r="94" spans="7:7" ht="14.25" customHeight="1">
       <c r="G94" s="3"/>
     </row>
-    <row r="95" ht="14.25" customHeight="1">
+    <row r="95" spans="7:7" ht="14.25" customHeight="1">
       <c r="G95" s="3"/>
     </row>
-    <row r="96" ht="14.25" customHeight="1">
+    <row r="96" spans="7:7" ht="14.25" customHeight="1">
       <c r="G96" s="3"/>
     </row>
-    <row r="97" ht="14.25" customHeight="1">
+    <row r="97" spans="7:7" ht="14.25" customHeight="1">
       <c r="G97" s="3"/>
     </row>
-    <row r="98" ht="14.25" customHeight="1">
+    <row r="98" spans="7:7" ht="14.25" customHeight="1">
       <c r="G98" s="3"/>
     </row>
-    <row r="99" ht="14.25" customHeight="1">
+    <row r="99" spans="7:7" ht="14.25" customHeight="1">
       <c r="G99" s="3"/>
     </row>
-    <row r="100" ht="14.25" customHeight="1">
+    <row r="100" spans="7:7" ht="14.25" customHeight="1">
       <c r="G100" s="3"/>
     </row>
-    <row r="101" ht="14.25" customHeight="1">
+    <row r="101" spans="7:7" ht="14.25" customHeight="1">
       <c r="G101" s="3"/>
     </row>
-    <row r="102" ht="14.25" customHeight="1">
+    <row r="102" spans="7:7" ht="14.25" customHeight="1">
       <c r="G102" s="3"/>
     </row>
-    <row r="103" ht="14.25" customHeight="1">
+    <row r="103" spans="7:7" ht="14.25" customHeight="1">
       <c r="G103" s="3"/>
     </row>
-    <row r="104" ht="14.25" customHeight="1">
+    <row r="104" spans="7:7" ht="14.25" customHeight="1">
       <c r="G104" s="3"/>
     </row>
-    <row r="105" ht="14.25" customHeight="1">
+    <row r="105" spans="7:7" ht="14.25" customHeight="1">
       <c r="G105" s="3"/>
     </row>
-    <row r="106" ht="14.25" customHeight="1">
+    <row r="106" spans="7:7" ht="14.25" customHeight="1">
       <c r="G106" s="3"/>
     </row>
-    <row r="107" ht="14.25" customHeight="1">
+    <row r="107" spans="7:7" ht="14.25" customHeight="1">
       <c r="G107" s="3"/>
     </row>
-    <row r="108" ht="14.25" customHeight="1">
+    <row r="108" spans="7:7" ht="14.25" customHeight="1">
       <c r="G108" s="3"/>
     </row>
-    <row r="109" ht="14.25" customHeight="1">
+    <row r="109" spans="7:7" ht="14.25" customHeight="1">
       <c r="G109" s="3"/>
     </row>
-    <row r="110" ht="14.25" customHeight="1">
+    <row r="110" spans="7:7" ht="14.25" customHeight="1">
       <c r="G110" s="3"/>
     </row>
-    <row r="111" ht="14.25" customHeight="1">
+    <row r="111" spans="7:7" ht="14.25" customHeight="1">
       <c r="G111" s="3"/>
     </row>
-    <row r="112" ht="14.25" customHeight="1">
+    <row r="112" spans="7:7" ht="14.25" customHeight="1">
       <c r="G112" s="3"/>
     </row>
-    <row r="113" ht="14.25" customHeight="1">
+    <row r="113" spans="7:7" ht="14.25" customHeight="1">
       <c r="G113" s="3"/>
     </row>
-    <row r="114" ht="14.25" customHeight="1">
+    <row r="114" spans="7:7" ht="14.25" customHeight="1">
       <c r="G114" s="3"/>
     </row>
-    <row r="115" ht="14.25" customHeight="1">
+    <row r="115" spans="7:7" ht="14.25" customHeight="1">
       <c r="G115" s="3"/>
     </row>
-    <row r="116" ht="14.25" customHeight="1">
+    <row r="116" spans="7:7" ht="14.25" customHeight="1">
       <c r="G116" s="3"/>
     </row>
-    <row r="117" ht="14.25" customHeight="1">
+    <row r="117" spans="7:7" ht="14.25" customHeight="1">
       <c r="G117" s="3"/>
     </row>
-    <row r="118" ht="14.25" customHeight="1">
+    <row r="118" spans="7:7" ht="14.25" customHeight="1">
       <c r="G118" s="3"/>
     </row>
-    <row r="119" ht="14.25" customHeight="1">
+    <row r="119" spans="7:7" ht="14.25" customHeight="1">
       <c r="G119" s="3"/>
     </row>
-    <row r="120" ht="14.25" customHeight="1">
+    <row r="120" spans="7:7" ht="14.25" customHeight="1">
       <c r="G120" s="3"/>
     </row>
-    <row r="121" ht="14.25" customHeight="1">
+    <row r="121" spans="7:7" ht="14.25" customHeight="1">
       <c r="G121" s="3"/>
     </row>
-    <row r="122" ht="14.25" customHeight="1">
+    <row r="122" spans="7:7" ht="14.25" customHeight="1">
       <c r="G122" s="3"/>
     </row>
-    <row r="123" ht="14.25" customHeight="1">
+    <row r="123" spans="7:7" ht="14.25" customHeight="1">
       <c r="G123" s="3"/>
     </row>
-    <row r="124" ht="14.25" customHeight="1">
+    <row r="124" spans="7:7" ht="14.25" customHeight="1">
       <c r="G124" s="3"/>
     </row>
-    <row r="125" ht="14.25" customHeight="1">
+    <row r="125" spans="7:7" ht="14.25" customHeight="1">
       <c r="G125" s="3"/>
     </row>
-    <row r="126" ht="14.25" customHeight="1">
+    <row r="126" spans="7:7" ht="14.25" customHeight="1">
       <c r="G126" s="3"/>
     </row>
-    <row r="127" ht="14.25" customHeight="1">
+    <row r="127" spans="7:7" ht="14.25" customHeight="1">
       <c r="G127" s="3"/>
     </row>
-    <row r="128" ht="14.25" customHeight="1">
+    <row r="128" spans="7:7" ht="14.25" customHeight="1">
       <c r="G128" s="3"/>
     </row>
-    <row r="129" ht="14.25" customHeight="1">
+    <row r="129" spans="7:7" ht="14.25" customHeight="1">
       <c r="G129" s="3"/>
     </row>
-    <row r="130" ht="14.25" customHeight="1">
+    <row r="130" spans="7:7" ht="14.25" customHeight="1">
       <c r="G130" s="3"/>
     </row>
-    <row r="131" ht="14.25" customHeight="1">
+    <row r="131" spans="7:7" ht="14.25" customHeight="1">
       <c r="G131" s="3"/>
     </row>
-    <row r="132" ht="14.25" customHeight="1">
+    <row r="132" spans="7:7" ht="14.25" customHeight="1">
       <c r="G132" s="3"/>
     </row>
-    <row r="133" ht="14.25" customHeight="1">
+    <row r="133" spans="7:7" ht="14.25" customHeight="1">
       <c r="G133" s="3"/>
     </row>
-    <row r="134" ht="14.25" customHeight="1">
+    <row r="134" spans="7:7" ht="14.25" customHeight="1">
       <c r="G134" s="3"/>
     </row>
-    <row r="135" ht="14.25" customHeight="1">
+    <row r="135" spans="7:7" ht="14.25" customHeight="1">
       <c r="G135" s="3"/>
     </row>
-    <row r="136" ht="14.25" customHeight="1">
+    <row r="136" spans="7:7" ht="14.25" customHeight="1">
       <c r="G136" s="3"/>
     </row>
-    <row r="137" ht="14.25" customHeight="1">
+    <row r="137" spans="7:7" ht="14.25" customHeight="1">
       <c r="G137" s="3"/>
     </row>
-    <row r="138" ht="14.25" customHeight="1">
+    <row r="138" spans="7:7" ht="14.25" customHeight="1">
       <c r="G138" s="3"/>
     </row>
-    <row r="139" ht="14.25" customHeight="1">
+    <row r="139" spans="7:7" ht="14.25" customHeight="1">
       <c r="G139" s="3"/>
     </row>
-    <row r="140" ht="14.25" customHeight="1">
+    <row r="140" spans="7:7" ht="14.25" customHeight="1">
       <c r="G140" s="3"/>
     </row>
-    <row r="141" ht="14.25" customHeight="1">
+    <row r="141" spans="7:7" ht="14.25" customHeight="1">
       <c r="G141" s="3"/>
     </row>
-    <row r="142" ht="14.25" customHeight="1">
+    <row r="142" spans="7:7" ht="14.25" customHeight="1">
       <c r="G142" s="3"/>
     </row>
-    <row r="143" ht="14.25" customHeight="1">
+    <row r="143" spans="7:7" ht="14.25" customHeight="1">
       <c r="G143" s="3"/>
     </row>
-    <row r="144" ht="14.25" customHeight="1">
+    <row r="144" spans="7:7" ht="14.25" customHeight="1">
       <c r="G144" s="3"/>
     </row>
-    <row r="145" ht="14.25" customHeight="1">
+    <row r="145" spans="7:7" ht="14.25" customHeight="1">
       <c r="G145" s="3"/>
     </row>
-    <row r="146" ht="14.25" customHeight="1">
+    <row r="146" spans="7:7" ht="14.25" customHeight="1">
       <c r="G146" s="3"/>
     </row>
-    <row r="147" ht="14.25" customHeight="1">
+    <row r="147" spans="7:7" ht="14.25" customHeight="1">
       <c r="G147" s="3"/>
     </row>
-    <row r="148" ht="14.25" customHeight="1">
+    <row r="148" spans="7:7" ht="14.25" customHeight="1">
       <c r="G148" s="3"/>
     </row>
-    <row r="149" ht="14.25" customHeight="1">
+    <row r="149" spans="7:7" ht="14.25" customHeight="1">
       <c r="G149" s="3"/>
     </row>
-    <row r="150" ht="14.25" customHeight="1">
+    <row r="150" spans="7:7" ht="14.25" customHeight="1">
       <c r="G150" s="3"/>
     </row>
-    <row r="151" ht="14.25" customHeight="1">
+    <row r="151" spans="7:7" ht="14.25" customHeight="1">
       <c r="G151" s="3"/>
     </row>
-    <row r="152" ht="14.25" customHeight="1">
+    <row r="152" spans="7:7" ht="14.25" customHeight="1">
       <c r="G152" s="3"/>
     </row>
-    <row r="153" ht="14.25" customHeight="1">
+    <row r="153" spans="7:7" ht="14.25" customHeight="1">
       <c r="G153" s="3"/>
     </row>
-    <row r="154" ht="14.25" customHeight="1">
+    <row r="154" spans="7:7" ht="14.25" customHeight="1">
       <c r="G154" s="3"/>
     </row>
-    <row r="155" ht="14.25" customHeight="1">
+    <row r="155" spans="7:7" ht="14.25" customHeight="1">
       <c r="G155" s="3"/>
     </row>
-    <row r="156" ht="14.25" customHeight="1">
+    <row r="156" spans="7:7" ht="14.25" customHeight="1">
       <c r="G156" s="3"/>
     </row>
-    <row r="157" ht="14.25" customHeight="1">
+    <row r="157" spans="7:7" ht="14.25" customHeight="1">
       <c r="G157" s="3"/>
     </row>
-    <row r="158" ht="14.25" customHeight="1">
+    <row r="158" spans="7:7" ht="14.25" customHeight="1">
       <c r="G158" s="3"/>
     </row>
-    <row r="159" ht="14.25" customHeight="1">
+    <row r="159" spans="7:7" ht="14.25" customHeight="1">
       <c r="G159" s="3"/>
     </row>
-    <row r="160" ht="14.25" customHeight="1">
+    <row r="160" spans="7:7" ht="14.25" customHeight="1">
       <c r="G160" s="3"/>
     </row>
-    <row r="161" ht="14.25" customHeight="1">
+    <row r="161" spans="7:7" ht="14.25" customHeight="1">
       <c r="G161" s="3"/>
     </row>
-    <row r="162" ht="14.25" customHeight="1">
+    <row r="162" spans="7:7" ht="14.25" customHeight="1">
       <c r="G162" s="3"/>
     </row>
-    <row r="163" ht="14.25" customHeight="1">
+    <row r="163" spans="7:7" ht="14.25" customHeight="1">
       <c r="G163" s="3"/>
     </row>
-    <row r="164" ht="14.25" customHeight="1">
+    <row r="164" spans="7:7" ht="14.25" customHeight="1">
       <c r="G164" s="3"/>
     </row>
-    <row r="165" ht="14.25" customHeight="1">
+    <row r="165" spans="7:7" ht="14.25" customHeight="1">
       <c r="G165" s="3"/>
     </row>
-    <row r="166" ht="14.25" customHeight="1">
+    <row r="166" spans="7:7" ht="14.25" customHeight="1">
       <c r="G166" s="3"/>
     </row>
-    <row r="167" ht="14.25" customHeight="1">
+    <row r="167" spans="7:7" ht="14.25" customHeight="1">
       <c r="G167" s="3"/>
     </row>
-    <row r="168" ht="14.25" customHeight="1">
+    <row r="168" spans="7:7" ht="14.25" customHeight="1">
       <c r="G168" s="3"/>
     </row>
-    <row r="169" ht="14.25" customHeight="1">
+    <row r="169" spans="7:7" ht="14.25" customHeight="1">
       <c r="G169" s="3"/>
     </row>
-    <row r="170" ht="14.25" customHeight="1">
+    <row r="170" spans="7:7" ht="14.25" customHeight="1">
       <c r="G170" s="3"/>
     </row>
-    <row r="171" ht="14.25" customHeight="1">
+    <row r="171" spans="7:7" ht="14.25" customHeight="1">
       <c r="G171" s="3"/>
     </row>
-    <row r="172" ht="14.25" customHeight="1">
+    <row r="172" spans="7:7" ht="14.25" customHeight="1">
       <c r="G172" s="3"/>
     </row>
-    <row r="173" ht="14.25" customHeight="1">
+    <row r="173" spans="7:7" ht="14.25" customHeight="1">
       <c r="G173" s="3"/>
     </row>
-    <row r="174" ht="14.25" customHeight="1">
+    <row r="174" spans="7:7" ht="14.25" customHeight="1">
       <c r="G174" s="3"/>
     </row>
-    <row r="175" ht="14.25" customHeight="1">
+    <row r="175" spans="7:7" ht="14.25" customHeight="1">
       <c r="G175" s="3"/>
     </row>
-    <row r="176" ht="14.25" customHeight="1">
+    <row r="176" spans="7:7" ht="14.25" customHeight="1">
       <c r="G176" s="3"/>
     </row>
-    <row r="177" ht="14.25" customHeight="1">
+    <row r="177" spans="7:7" ht="14.25" customHeight="1">
       <c r="G177" s="3"/>
     </row>
-    <row r="178" ht="14.25" customHeight="1">
+    <row r="178" spans="7:7" ht="14.25" customHeight="1">
       <c r="G178" s="3"/>
     </row>
-    <row r="179" ht="14.25" customHeight="1">
+    <row r="179" spans="7:7" ht="14.25" customHeight="1">
       <c r="G179" s="3"/>
     </row>
-    <row r="180" ht="14.25" customHeight="1">
+    <row r="180" spans="7:7" ht="14.25" customHeight="1">
       <c r="G180" s="3"/>
     </row>
-    <row r="181" ht="14.25" customHeight="1">
+    <row r="181" spans="7:7" ht="14.25" customHeight="1">
       <c r="G181" s="3"/>
     </row>
-    <row r="182" ht="14.25" customHeight="1">
+    <row r="182" spans="7:7" ht="14.25" customHeight="1">
       <c r="G182" s="3"/>
     </row>
-    <row r="183" ht="14.25" customHeight="1">
+    <row r="183" spans="7:7" ht="14.25" customHeight="1">
       <c r="G183" s="3"/>
     </row>
-    <row r="184" ht="14.25" customHeight="1">
+    <row r="184" spans="7:7" ht="14.25" customHeight="1">
       <c r="G184" s="3"/>
     </row>
-    <row r="185" ht="14.25" customHeight="1">
+    <row r="185" spans="7:7" ht="14.25" customHeight="1">
       <c r="G185" s="3"/>
     </row>
-    <row r="186" ht="14.25" customHeight="1">
+    <row r="186" spans="7:7" ht="14.25" customHeight="1">
       <c r="G186" s="3"/>
     </row>
-    <row r="187" ht="14.25" customHeight="1">
+    <row r="187" spans="7:7" ht="14.25" customHeight="1">
       <c r="G187" s="3"/>
     </row>
-    <row r="188" ht="14.25" customHeight="1">
+    <row r="188" spans="7:7" ht="14.25" customHeight="1">
       <c r="G188" s="3"/>
     </row>
-    <row r="189" ht="14.25" customHeight="1">
+    <row r="189" spans="7:7" ht="14.25" customHeight="1">
       <c r="G189" s="3"/>
     </row>
-    <row r="190" ht="14.25" customHeight="1">
+    <row r="190" spans="7:7" ht="14.25" customHeight="1">
       <c r="G190" s="3"/>
     </row>
-    <row r="191" ht="14.25" customHeight="1">
+    <row r="191" spans="7:7" ht="14.25" customHeight="1">
       <c r="G191" s="3"/>
     </row>
-    <row r="192" ht="14.25" customHeight="1">
+    <row r="192" spans="7:7" ht="14.25" customHeight="1">
       <c r="G192" s="3"/>
     </row>
-    <row r="193" ht="14.25" customHeight="1">
+    <row r="193" spans="7:7" ht="14.25" customHeight="1">
       <c r="G193" s="3"/>
     </row>
-    <row r="194" ht="14.25" customHeight="1">
+    <row r="194" spans="7:7" ht="14.25" customHeight="1">
       <c r="G194" s="3"/>
     </row>
-    <row r="195" ht="14.25" customHeight="1">
+    <row r="195" spans="7:7" ht="14.25" customHeight="1">
       <c r="G195" s="3"/>
     </row>
-    <row r="196" ht="14.25" customHeight="1">
+    <row r="196" spans="7:7" ht="14.25" customHeight="1">
       <c r="G196" s="3"/>
     </row>
-    <row r="197" ht="14.25" customHeight="1">
+    <row r="197" spans="7:7" ht="14.25" customHeight="1">
       <c r="G197" s="3"/>
     </row>
-    <row r="198" ht="14.25" customHeight="1">
+    <row r="198" spans="7:7" ht="14.25" customHeight="1">
       <c r="G198" s="3"/>
     </row>
-    <row r="199" ht="14.25" customHeight="1">
+    <row r="199" spans="7:7" ht="14.25" customHeight="1">
       <c r="G199" s="3"/>
     </row>
-    <row r="200" ht="14.25" customHeight="1">
+    <row r="200" spans="7:7" ht="14.25" customHeight="1">
       <c r="G200" s="3"/>
     </row>
-    <row r="201" ht="14.25" customHeight="1">
+    <row r="201" spans="7:7" ht="14.25" customHeight="1">
       <c r="G201" s="3"/>
     </row>
-    <row r="202" ht="14.25" customHeight="1">
+    <row r="202" spans="7:7" ht="14.25" customHeight="1">
       <c r="G202" s="3"/>
     </row>
-    <row r="203" ht="14.25" customHeight="1">
+    <row r="203" spans="7:7" ht="14.25" customHeight="1">
       <c r="G203" s="3"/>
     </row>
-    <row r="204" ht="14.25" customHeight="1">
+    <row r="204" spans="7:7" ht="14.25" customHeight="1">
       <c r="G204" s="3"/>
     </row>
-    <row r="205" ht="14.25" customHeight="1">
+    <row r="205" spans="7:7" ht="14.25" customHeight="1">
       <c r="G205" s="3"/>
     </row>
-    <row r="206" ht="14.25" customHeight="1">
+    <row r="206" spans="7:7" ht="14.25" customHeight="1">
       <c r="G206" s="3"/>
     </row>
-    <row r="207" ht="14.25" customHeight="1">
+    <row r="207" spans="7:7" ht="14.25" customHeight="1">
       <c r="G207" s="3"/>
     </row>
-    <row r="208" ht="14.25" customHeight="1">
+    <row r="208" spans="7:7" ht="14.25" customHeight="1">
       <c r="G208" s="3"/>
     </row>
-    <row r="209" ht="14.25" customHeight="1">
+    <row r="209" spans="7:7" ht="14.25" customHeight="1">
       <c r="G209" s="3"/>
     </row>
-    <row r="210" ht="14.25" customHeight="1">
+    <row r="210" spans="7:7" ht="14.25" customHeight="1">
       <c r="G210" s="3"/>
     </row>
-    <row r="211" ht="14.25" customHeight="1">
+    <row r="211" spans="7:7" ht="14.25" customHeight="1">
       <c r="G211" s="3"/>
     </row>
-    <row r="212" ht="14.25" customHeight="1">
+    <row r="212" spans="7:7" ht="14.25" customHeight="1">
       <c r="G212" s="3"/>
     </row>
-    <row r="213" ht="14.25" customHeight="1">
+    <row r="213" spans="7:7" ht="14.25" customHeight="1">
       <c r="G213" s="3"/>
     </row>
-    <row r="214" ht="14.25" customHeight="1">
+    <row r="214" spans="7:7" ht="14.25" customHeight="1">
       <c r="G214" s="3"/>
     </row>
-    <row r="215" ht="14.25" customHeight="1">
+    <row r="215" spans="7:7" ht="14.25" customHeight="1">
       <c r="G215" s="3"/>
     </row>
-    <row r="216" ht="14.25" customHeight="1">
+    <row r="216" spans="7:7" ht="14.25" customHeight="1">
       <c r="G216" s="3"/>
     </row>
-    <row r="217" ht="14.25" customHeight="1">
+    <row r="217" spans="7:7" ht="14.25" customHeight="1">
       <c r="G217" s="3"/>
     </row>
-    <row r="218" ht="14.25" customHeight="1">
+    <row r="218" spans="7:7" ht="14.25" customHeight="1">
       <c r="G218" s="3"/>
     </row>
-    <row r="219" ht="14.25" customHeight="1">
+    <row r="219" spans="7:7" ht="14.25" customHeight="1">
       <c r="G219" s="3"/>
     </row>
-    <row r="220" ht="14.25" customHeight="1">
+    <row r="220" spans="7:7" ht="14.25" customHeight="1">
       <c r="G220" s="3"/>
     </row>
-    <row r="221" ht="14.25" customHeight="1">
+    <row r="221" spans="7:7" ht="14.25" customHeight="1">
       <c r="G221" s="3"/>
     </row>
-    <row r="222" ht="14.25" customHeight="1">
+    <row r="222" spans="7:7" ht="14.25" customHeight="1">
       <c r="G222" s="3"/>
     </row>
-    <row r="223" ht="14.25" customHeight="1">
+    <row r="223" spans="7:7" ht="14.25" customHeight="1">
       <c r="G223" s="3"/>
     </row>
-    <row r="224" ht="14.25" customHeight="1">
+    <row r="224" spans="7:7" ht="14.25" customHeight="1">
       <c r="G224" s="3"/>
     </row>
-    <row r="225" ht="14.25" customHeight="1">
+    <row r="225" spans="7:7" ht="14.25" customHeight="1">
       <c r="G225" s="3"/>
     </row>
-    <row r="226" ht="14.25" customHeight="1">
+    <row r="226" spans="7:7" ht="14.25" customHeight="1">
       <c r="G226" s="3"/>
     </row>
-    <row r="227" ht="14.25" customHeight="1">
+    <row r="227" spans="7:7" ht="14.25" customHeight="1">
       <c r="G227" s="3"/>
     </row>
-    <row r="228" ht="14.25" customHeight="1">
+    <row r="228" spans="7:7" ht="14.25" customHeight="1">
       <c r="G228" s="3"/>
     </row>
-    <row r="229" ht="14.25" customHeight="1">
+    <row r="229" spans="7:7" ht="14.25" customHeight="1">
       <c r="G229" s="3"/>
     </row>
-    <row r="230" ht="14.25" customHeight="1">
+    <row r="230" spans="7:7" ht="14.25" customHeight="1">
       <c r="G230" s="3"/>
     </row>
-    <row r="231" ht="14.25" customHeight="1">
+    <row r="231" spans="7:7" ht="14.25" customHeight="1">
       <c r="G231" s="3"/>
     </row>
-    <row r="232" ht="14.25" customHeight="1">
+    <row r="232" spans="7:7" ht="14.25" customHeight="1">
       <c r="G232" s="3"/>
     </row>
-    <row r="233" ht="14.25" customHeight="1">
+    <row r="233" spans="7:7" ht="14.25" customHeight="1">
       <c r="G233" s="3"/>
     </row>
-    <row r="234" ht="14.25" customHeight="1">
+    <row r="234" spans="7:7" ht="14.25" customHeight="1">
       <c r="G234" s="3"/>
     </row>
-    <row r="235" ht="14.25" customHeight="1">
+    <row r="235" spans="7:7" ht="14.25" customHeight="1">
       <c r="G235" s="3"/>
     </row>
-    <row r="236" ht="14.25" customHeight="1">
+    <row r="236" spans="7:7" ht="14.25" customHeight="1">
       <c r="G236" s="3"/>
     </row>
-    <row r="237" ht="14.25" customHeight="1">
+    <row r="237" spans="7:7" ht="14.25" customHeight="1">
       <c r="G237" s="3"/>
     </row>
-    <row r="238" ht="14.25" customHeight="1">
+    <row r="238" spans="7:7" ht="14.25" customHeight="1">
       <c r="G238" s="3"/>
     </row>
-    <row r="239" ht="14.25" customHeight="1">
+    <row r="239" spans="7:7" ht="14.25" customHeight="1">
       <c r="G239" s="3"/>
     </row>
-    <row r="240" ht="14.25" customHeight="1">
+    <row r="240" spans="7:7" ht="14.25" customHeight="1">
       <c r="G240" s="3"/>
     </row>
-    <row r="241" ht="14.25" customHeight="1">
+    <row r="241" spans="7:7" ht="14.25" customHeight="1">
       <c r="G241" s="3"/>
     </row>
-    <row r="242" ht="14.25" customHeight="1">
+    <row r="242" spans="7:7" ht="14.25" customHeight="1">
       <c r="G242" s="3"/>
     </row>
-    <row r="243" ht="14.25" customHeight="1">
+    <row r="243" spans="7:7" ht="14.25" customHeight="1">
       <c r="G243" s="3"/>
     </row>
-    <row r="244" ht="14.25" customHeight="1">
+    <row r="244" spans="7:7" ht="14.25" customHeight="1">
       <c r="G244" s="3"/>
     </row>
-    <row r="245" ht="14.25" customHeight="1">
+    <row r="245" spans="7:7" ht="14.25" customHeight="1">
       <c r="G245" s="3"/>
     </row>
-    <row r="246" ht="14.25" customHeight="1">
+    <row r="246" spans="7:7" ht="14.25" customHeight="1">
       <c r="G246" s="3"/>
     </row>
-    <row r="247" ht="14.25" customHeight="1">
+    <row r="247" spans="7:7" ht="14.25" customHeight="1">
       <c r="G247" s="3"/>
     </row>
-    <row r="248" ht="14.25" customHeight="1">
+    <row r="248" spans="7:7" ht="14.25" customHeight="1">
       <c r="G248" s="3"/>
     </row>
-    <row r="249" ht="14.25" customHeight="1">
+    <row r="249" spans="7:7" ht="14.25" customHeight="1">
       <c r="G249" s="3"/>
     </row>
-    <row r="250" ht="14.25" customHeight="1">
+    <row r="250" spans="7:7" ht="14.25" customHeight="1">
       <c r="G250" s="3"/>
     </row>
-    <row r="251" ht="14.25" customHeight="1">
+    <row r="251" spans="7:7" ht="14.25" customHeight="1">
       <c r="G251" s="3"/>
     </row>
-    <row r="252" ht="14.25" customHeight="1">
+    <row r="252" spans="7:7" ht="14.25" customHeight="1">
       <c r="G252" s="3"/>
     </row>
-    <row r="253" ht="14.25" customHeight="1">
+    <row r="253" spans="7:7" ht="14.25" customHeight="1">
       <c r="G253" s="3"/>
     </row>
-    <row r="254" ht="14.25" customHeight="1">
+    <row r="254" spans="7:7" ht="14.25" customHeight="1">
       <c r="G254" s="3"/>
     </row>
-    <row r="255" ht="14.25" customHeight="1">
+    <row r="255" spans="7:7" ht="14.25" customHeight="1">
       <c r="G255" s="3"/>
     </row>
-    <row r="256" ht="14.25" customHeight="1">
+    <row r="256" spans="7:7" ht="14.25" customHeight="1">
       <c r="G256" s="3"/>
     </row>
-    <row r="257" ht="14.25" customHeight="1">
+    <row r="257" spans="7:7" ht="14.25" customHeight="1">
       <c r="G257" s="3"/>
     </row>
-    <row r="258" ht="14.25" customHeight="1">
+    <row r="258" spans="7:7" ht="14.25" customHeight="1">
       <c r="G258" s="3"/>
     </row>
-    <row r="259" ht="14.25" customHeight="1">
+    <row r="259" spans="7:7" ht="14.25" customHeight="1">
       <c r="G259" s="3"/>
     </row>
-    <row r="260" ht="14.25" customHeight="1">
+    <row r="260" spans="7:7" ht="14.25" customHeight="1">
       <c r="G260" s="3"/>
     </row>
-    <row r="261" ht="14.25" customHeight="1">
+    <row r="261" spans="7:7" ht="14.25" customHeight="1">
       <c r="G261" s="3"/>
     </row>
-    <row r="262" ht="14.25" customHeight="1">
+    <row r="262" spans="7:7" ht="14.25" customHeight="1">
       <c r="G262" s="3"/>
     </row>
-    <row r="263" ht="14.25" customHeight="1">
+    <row r="263" spans="7:7" ht="14.25" customHeight="1">
       <c r="G263" s="3"/>
     </row>
-    <row r="264" ht="14.25" customHeight="1">
+    <row r="264" spans="7:7" ht="14.25" customHeight="1">
       <c r="G264" s="3"/>
     </row>
-    <row r="265" ht="14.25" customHeight="1">
+    <row r="265" spans="7:7" ht="14.25" customHeight="1">
       <c r="G265" s="3"/>
     </row>
-    <row r="266" ht="14.25" customHeight="1">
+    <row r="266" spans="7:7" ht="14.25" customHeight="1">
       <c r="G266" s="3"/>
     </row>
-    <row r="267" ht="14.25" customHeight="1">
+    <row r="267" spans="7:7" ht="14.25" customHeight="1">
       <c r="G267" s="3"/>
     </row>
-    <row r="268" ht="14.25" customHeight="1">
+    <row r="268" spans="7:7" ht="14.25" customHeight="1">
       <c r="G268" s="3"/>
     </row>
-    <row r="269" ht="14.25" customHeight="1">
+    <row r="269" spans="7:7" ht="14.25" customHeight="1">
       <c r="G269" s="3"/>
     </row>
-    <row r="270" ht="14.25" customHeight="1">
+    <row r="270" spans="7:7" ht="14.25" customHeight="1">
       <c r="G270" s="3"/>
     </row>
-    <row r="271" ht="14.25" customHeight="1">
+    <row r="271" spans="7:7" ht="14.25" customHeight="1">
       <c r="G271" s="3"/>
     </row>
-    <row r="272" ht="14.25" customHeight="1">
+    <row r="272" spans="7:7" ht="14.25" customHeight="1">
       <c r="G272" s="3"/>
     </row>
-    <row r="273" ht="14.25" customHeight="1">
+    <row r="273" spans="7:7" ht="14.25" customHeight="1">
       <c r="G273" s="3"/>
     </row>
-    <row r="274" ht="14.25" customHeight="1">
+    <row r="274" spans="7:7" ht="14.25" customHeight="1">
       <c r="G274" s="3"/>
     </row>
-    <row r="275" ht="14.25" customHeight="1">
+    <row r="275" spans="7:7" ht="14.25" customHeight="1">
       <c r="G275" s="3"/>
     </row>
-    <row r="276" ht="14.25" customHeight="1">
+    <row r="276" spans="7:7" ht="14.25" customHeight="1">
       <c r="G276" s="3"/>
     </row>
-    <row r="277" ht="14.25" customHeight="1">
+    <row r="277" spans="7:7" ht="14.25" customHeight="1">
       <c r="G277" s="3"/>
     </row>
-    <row r="278" ht="14.25" customHeight="1">
+    <row r="278" spans="7:7" ht="14.25" customHeight="1">
       <c r="G278" s="3"/>
     </row>
-    <row r="279" ht="14.25" customHeight="1">
+    <row r="279" spans="7:7" ht="14.25" customHeight="1">
       <c r="G279" s="3"/>
     </row>
-    <row r="280" ht="14.25" customHeight="1">
+    <row r="280" spans="7:7" ht="14.25" customHeight="1">
       <c r="G280" s="3"/>
     </row>
-    <row r="281" ht="14.25" customHeight="1">
+    <row r="281" spans="7:7" ht="14.25" customHeight="1">
       <c r="G281" s="3"/>
     </row>
-    <row r="282" ht="14.25" customHeight="1">
+    <row r="282" spans="7:7" ht="14.25" customHeight="1">
       <c r="G282" s="3"/>
     </row>
-    <row r="283" ht="14.25" customHeight="1">
+    <row r="283" spans="7:7" ht="14.25" customHeight="1">
       <c r="G283" s="3"/>
     </row>
-    <row r="284" ht="14.25" customHeight="1">
+    <row r="284" spans="7:7" ht="14.25" customHeight="1">
       <c r="G284" s="3"/>
     </row>
-    <row r="285" ht="14.25" customHeight="1">
+    <row r="285" spans="7:7" ht="14.25" customHeight="1">
       <c r="G285" s="3"/>
     </row>
-    <row r="286" ht="14.25" customHeight="1">
+    <row r="286" spans="7:7" ht="14.25" customHeight="1">
       <c r="G286" s="3"/>
     </row>
-    <row r="287" ht="14.25" customHeight="1">
+    <row r="287" spans="7:7" ht="14.25" customHeight="1">
       <c r="G287" s="3"/>
     </row>
-    <row r="288" ht="14.25" customHeight="1">
+    <row r="288" spans="7:7" ht="14.25" customHeight="1">
       <c r="G288" s="3"/>
     </row>
-    <row r="289" ht="14.25" customHeight="1">
+    <row r="289" spans="7:7" ht="14.25" customHeight="1">
       <c r="G289" s="3"/>
     </row>
-    <row r="290" ht="14.25" customHeight="1">
+    <row r="290" spans="7:7" ht="14.25" customHeight="1">
       <c r="G290" s="3"/>
     </row>
-    <row r="291" ht="14.25" customHeight="1">
+    <row r="291" spans="7:7" ht="14.25" customHeight="1">
       <c r="G291" s="3"/>
     </row>
-    <row r="292" ht="14.25" customHeight="1">
+    <row r="292" spans="7:7" ht="14.25" customHeight="1">
       <c r="G292" s="3"/>
     </row>
-    <row r="293" ht="14.25" customHeight="1">
+    <row r="293" spans="7:7" ht="14.25" customHeight="1">
       <c r="G293" s="3"/>
     </row>
-    <row r="294" ht="14.25" customHeight="1">
+    <row r="294" spans="7:7" ht="14.25" customHeight="1">
       <c r="G294" s="3"/>
     </row>
-    <row r="295" ht="14.25" customHeight="1">
+    <row r="295" spans="7:7" ht="14.25" customHeight="1">
       <c r="G295" s="3"/>
     </row>
-    <row r="296" ht="14.25" customHeight="1">
+    <row r="296" spans="7:7" ht="14.25" customHeight="1">
       <c r="G296" s="3"/>
     </row>
-    <row r="297" ht="14.25" customHeight="1">
+    <row r="297" spans="7:7" ht="14.25" customHeight="1">
       <c r="G297" s="3"/>
     </row>
-    <row r="298" ht="14.25" customHeight="1">
+    <row r="298" spans="7:7" ht="14.25" customHeight="1">
       <c r="G298" s="3"/>
     </row>
-    <row r="299" ht="14.25" customHeight="1">
+    <row r="299" spans="7:7" ht="14.25" customHeight="1">
       <c r="G299" s="3"/>
     </row>
-    <row r="300" ht="14.25" customHeight="1">
+    <row r="300" spans="7:7" ht="14.25" customHeight="1">
       <c r="G300" s="3"/>
     </row>
-    <row r="301" ht="14.25" customHeight="1">
+    <row r="301" spans="7:7" ht="14.25" customHeight="1">
       <c r="G301" s="3"/>
     </row>
-    <row r="302" ht="14.25" customHeight="1">
+    <row r="302" spans="7:7" ht="14.25" customHeight="1">
       <c r="G302" s="3"/>
     </row>
-    <row r="303" ht="14.25" customHeight="1">
+    <row r="303" spans="7:7" ht="14.25" customHeight="1">
       <c r="G303" s="3"/>
     </row>
-    <row r="304" ht="14.25" customHeight="1">
+    <row r="304" spans="7:7" ht="14.25" customHeight="1">
       <c r="G304" s="3"/>
     </row>
-    <row r="305" ht="14.25" customHeight="1">
+    <row r="305" spans="7:7" ht="14.25" customHeight="1">
       <c r="G305" s="3"/>
     </row>
-    <row r="306" ht="14.25" customHeight="1">
+    <row r="306" spans="7:7" ht="14.25" customHeight="1">
       <c r="G306" s="3"/>
     </row>
-    <row r="307" ht="14.25" customHeight="1">
+    <row r="307" spans="7:7" ht="14.25" customHeight="1">
       <c r="G307" s="3"/>
     </row>
-    <row r="308" ht="14.25" customHeight="1">
+    <row r="308" spans="7:7" ht="14.25" customHeight="1">
       <c r="G308" s="3"/>
     </row>
-    <row r="309" ht="14.25" customHeight="1">
+    <row r="309" spans="7:7" ht="14.25" customHeight="1">
       <c r="G309" s="3"/>
     </row>
-    <row r="310" ht="14.25" customHeight="1">
+    <row r="310" spans="7:7" ht="14.25" customHeight="1">
       <c r="G310" s="3"/>
     </row>
-    <row r="311" ht="14.25" customHeight="1">
+    <row r="311" spans="7:7" ht="14.25" customHeight="1">
       <c r="G311" s="3"/>
     </row>
-    <row r="312" ht="14.25" customHeight="1">
+    <row r="312" spans="7:7" ht="14.25" customHeight="1">
       <c r="G312" s="3"/>
     </row>
-    <row r="313" ht="14.25" customHeight="1">
+    <row r="313" spans="7:7" ht="14.25" customHeight="1">
       <c r="G313" s="3"/>
     </row>
-    <row r="314" ht="14.25" customHeight="1">
+    <row r="314" spans="7:7" ht="14.25" customHeight="1">
       <c r="G314" s="3"/>
     </row>
-    <row r="315" ht="14.25" customHeight="1">
+    <row r="315" spans="7:7" ht="14.25" customHeight="1">
       <c r="G315" s="3"/>
     </row>
-    <row r="316" ht="14.25" customHeight="1">
+    <row r="316" spans="7:7" ht="14.25" customHeight="1">
       <c r="G316" s="3"/>
     </row>
-    <row r="317" ht="14.25" customHeight="1">
+    <row r="317" spans="7:7" ht="14.25" customHeight="1">
       <c r="G317" s="3"/>
     </row>
-    <row r="318" ht="14.25" customHeight="1">
+    <row r="318" spans="7:7" ht="14.25" customHeight="1">
       <c r="G318" s="3"/>
     </row>
-    <row r="319" ht="14.25" customHeight="1">
+    <row r="319" spans="7:7" ht="14.25" customHeight="1">
       <c r="G319" s="3"/>
     </row>
-    <row r="320" ht="14.25" customHeight="1">
+    <row r="320" spans="7:7" ht="14.25" customHeight="1">
       <c r="G320" s="3"/>
     </row>
-    <row r="321" ht="14.25" customHeight="1">
+    <row r="321" spans="7:7" ht="14.25" customHeight="1">
       <c r="G321" s="3"/>
     </row>
-    <row r="322" ht="14.25" customHeight="1">
+    <row r="322" spans="7:7" ht="14.25" customHeight="1">
       <c r="G322" s="3"/>
     </row>
-    <row r="323" ht="14.25" customHeight="1">
+    <row r="323" spans="7:7" ht="14.25" customHeight="1">
       <c r="G323" s="3"/>
     </row>
-    <row r="324" ht="14.25" customHeight="1">
+    <row r="324" spans="7:7" ht="14.25" customHeight="1">
       <c r="G324" s="3"/>
     </row>
-    <row r="325" ht="14.25" customHeight="1">
+    <row r="325" spans="7:7" ht="14.25" customHeight="1">
       <c r="G325" s="3"/>
     </row>
-    <row r="326" ht="14.25" customHeight="1">
+    <row r="326" spans="7:7" ht="14.25" customHeight="1">
       <c r="G326" s="3"/>
     </row>
-    <row r="327" ht="14.25" customHeight="1">
+    <row r="327" spans="7:7" ht="14.25" customHeight="1">
       <c r="G327" s="3"/>
     </row>
-    <row r="328" ht="14.25" customHeight="1">
+    <row r="328" spans="7:7" ht="14.25" customHeight="1">
       <c r="G328" s="3"/>
     </row>
-    <row r="329" ht="14.25" customHeight="1">
+    <row r="329" spans="7:7" ht="14.25" customHeight="1">
       <c r="G329" s="3"/>
     </row>
-    <row r="330" ht="14.25" customHeight="1">
+    <row r="330" spans="7:7" ht="14.25" customHeight="1">
       <c r="G330" s="3"/>
     </row>
-    <row r="331" ht="14.25" customHeight="1">
+    <row r="331" spans="7:7" ht="14.25" customHeight="1">
       <c r="G331" s="3"/>
     </row>
-    <row r="332" ht="14.25" customHeight="1">
+    <row r="332" spans="7:7" ht="14.25" customHeight="1">
       <c r="G332" s="3"/>
     </row>
-    <row r="333" ht="14.25" customHeight="1">
+    <row r="333" spans="7:7" ht="14.25" customHeight="1">
       <c r="G333" s="3"/>
     </row>
-    <row r="334" ht="14.25" customHeight="1">
+    <row r="334" spans="7:7" ht="14.25" customHeight="1">
       <c r="G334" s="3"/>
     </row>
-    <row r="335" ht="14.25" customHeight="1">
+    <row r="335" spans="7:7" ht="14.25" customHeight="1">
       <c r="G335" s="3"/>
     </row>
-    <row r="336" ht="14.25" customHeight="1">
+    <row r="336" spans="7:7" ht="14.25" customHeight="1">
       <c r="G336" s="3"/>
     </row>
-    <row r="337" ht="14.25" customHeight="1">
+    <row r="337" spans="7:7" ht="14.25" customHeight="1">
       <c r="G337" s="3"/>
     </row>
-    <row r="338" ht="14.25" customHeight="1">
+    <row r="338" spans="7:7" ht="14.25" customHeight="1">
       <c r="G338" s="3"/>
     </row>
-    <row r="339" ht="14.25" customHeight="1">
+    <row r="339" spans="7:7" ht="14.25" customHeight="1">
       <c r="G339" s="3"/>
     </row>
-    <row r="340" ht="14.25" customHeight="1">
+    <row r="340" spans="7:7" ht="14.25" customHeight="1">
       <c r="G340" s="3"/>
     </row>
-    <row r="341" ht="14.25" customHeight="1">
+    <row r="341" spans="7:7" ht="14.25" customHeight="1">
       <c r="G341" s="3"/>
     </row>
-    <row r="342" ht="14.25" customHeight="1">
+    <row r="342" spans="7:7" ht="14.25" customHeight="1">
       <c r="G342" s="3"/>
     </row>
-    <row r="343" ht="14.25" customHeight="1">
+    <row r="343" spans="7:7" ht="14.25" customHeight="1">
       <c r="G343" s="3"/>
     </row>
-    <row r="344" ht="14.25" customHeight="1">
+    <row r="344" spans="7:7" ht="14.25" customHeight="1">
       <c r="G344" s="3"/>
     </row>
-    <row r="345" ht="14.25" customHeight="1">
+    <row r="345" spans="7:7" ht="14.25" customHeight="1">
       <c r="G345" s="3"/>
     </row>
-    <row r="346" ht="14.25" customHeight="1">
+    <row r="346" spans="7:7" ht="14.25" customHeight="1">
       <c r="G346" s="3"/>
     </row>
-    <row r="347" ht="14.25" customHeight="1">
+    <row r="347" spans="7:7" ht="14.25" customHeight="1">
       <c r="G347" s="3"/>
     </row>
-    <row r="348" ht="14.25" customHeight="1">
+    <row r="348" spans="7:7" ht="14.25" customHeight="1">
       <c r="G348" s="3"/>
     </row>
-    <row r="349" ht="14.25" customHeight="1">
+    <row r="349" spans="7:7" ht="14.25" customHeight="1">
       <c r="G349" s="3"/>
     </row>
-    <row r="350" ht="14.25" customHeight="1">
+    <row r="350" spans="7:7" ht="14.25" customHeight="1">
       <c r="G350" s="3"/>
     </row>
-    <row r="351" ht="14.25" customHeight="1">
+    <row r="351" spans="7:7" ht="14.25" customHeight="1">
       <c r="G351" s="3"/>
     </row>
-    <row r="352" ht="14.25" customHeight="1">
+    <row r="352" spans="7:7" ht="14.25" customHeight="1">
       <c r="G352" s="3"/>
     </row>
-    <row r="353" ht="14.25" customHeight="1">
+    <row r="353" spans="7:7" ht="14.25" customHeight="1">
       <c r="G353" s="3"/>
     </row>
-    <row r="354" ht="14.25" customHeight="1">
+    <row r="354" spans="7:7" ht="14.25" customHeight="1">
       <c r="G354" s="3"/>
     </row>
-    <row r="355" ht="14.25" customHeight="1">
+    <row r="355" spans="7:7" ht="14.25" customHeight="1">
       <c r="G355" s="3"/>
     </row>
-    <row r="356" ht="14.25" customHeight="1">
+    <row r="356" spans="7:7" ht="14.25" customHeight="1">
       <c r="G356" s="3"/>
     </row>
-    <row r="357" ht="14.25" customHeight="1">
+    <row r="357" spans="7:7" ht="14.25" customHeight="1">
       <c r="G357" s="3"/>
     </row>
-    <row r="358" ht="14.25" customHeight="1">
+    <row r="358" spans="7:7" ht="14.25" customHeight="1">
       <c r="G358" s="3"/>
     </row>
-    <row r="359" ht="14.25" customHeight="1">
+    <row r="359" spans="7:7" ht="14.25" customHeight="1">
       <c r="G359" s="3"/>
     </row>
-    <row r="360" ht="14.25" customHeight="1">
+    <row r="360" spans="7:7" ht="14.25" customHeight="1">
       <c r="G360" s="3"/>
     </row>
-    <row r="361" ht="14.25" customHeight="1">
+    <row r="361" spans="7:7" ht="14.25" customHeight="1">
       <c r="G361" s="3"/>
     </row>
-    <row r="362" ht="14.25" customHeight="1">
+    <row r="362" spans="7:7" ht="14.25" customHeight="1">
       <c r="G362" s="3"/>
     </row>
-    <row r="363" ht="14.25" customHeight="1">
+    <row r="363" spans="7:7" ht="14.25" customHeight="1">
       <c r="G363" s="3"/>
     </row>
-    <row r="364" ht="14.25" customHeight="1">
+    <row r="364" spans="7:7" ht="14.25" customHeight="1">
       <c r="G364" s="3"/>
     </row>
-    <row r="365" ht="14.25" customHeight="1">
+    <row r="365" spans="7:7" ht="14.25" customHeight="1">
       <c r="G365" s="3"/>
     </row>
-    <row r="366" ht="14.25" customHeight="1">
+    <row r="366" spans="7:7" ht="14.25" customHeight="1">
       <c r="G366" s="3"/>
     </row>
-    <row r="367" ht="14.25" customHeight="1">
+    <row r="367" spans="7:7" ht="14.25" customHeight="1">
       <c r="G367" s="3"/>
     </row>
-    <row r="368" ht="14.25" customHeight="1">
+    <row r="368" spans="7:7" ht="14.25" customHeight="1">
       <c r="G368" s="3"/>
     </row>
-    <row r="369" ht="14.25" customHeight="1">
+    <row r="369" spans="7:7" ht="14.25" customHeight="1">
       <c r="G369" s="3"/>
     </row>
-    <row r="370" ht="14.25" customHeight="1">
+    <row r="370" spans="7:7" ht="14.25" customHeight="1">
       <c r="G370" s="3"/>
     </row>
-    <row r="371" ht="14.25" customHeight="1">
+    <row r="371" spans="7:7" ht="14.25" customHeight="1">
       <c r="G371" s="3"/>
     </row>
-    <row r="372" ht="14.25" customHeight="1">
+    <row r="372" spans="7:7" ht="14.25" customHeight="1">
       <c r="G372" s="3"/>
     </row>
-    <row r="373" ht="14.25" customHeight="1">
+    <row r="373" spans="7:7" ht="14.25" customHeight="1">
       <c r="G373" s="3"/>
     </row>
-    <row r="374" ht="14.25" customHeight="1">
+    <row r="374" spans="7:7" ht="14.25" customHeight="1">
       <c r="G374" s="3"/>
     </row>
-    <row r="375" ht="14.25" customHeight="1">
+    <row r="375" spans="7:7" ht="14.25" customHeight="1">
       <c r="G375" s="3"/>
     </row>
-    <row r="376" ht="14.25" customHeight="1">
+    <row r="376" spans="7:7" ht="14.25" customHeight="1">
       <c r="G376" s="3"/>
     </row>
-    <row r="377" ht="14.25" customHeight="1">
+    <row r="377" spans="7:7" ht="14.25" customHeight="1">
       <c r="G377" s="3"/>
     </row>
-    <row r="378" ht="14.25" customHeight="1">
+    <row r="378" spans="7:7" ht="14.25" customHeight="1">
       <c r="G378" s="3"/>
     </row>
-    <row r="379" ht="14.25" customHeight="1">
+    <row r="379" spans="7:7" ht="14.25" customHeight="1">
       <c r="G379" s="3"/>
     </row>
-    <row r="380" ht="14.25" customHeight="1">
+    <row r="380" spans="7:7" ht="14.25" customHeight="1">
       <c r="G380" s="3"/>
     </row>
-    <row r="381" ht="14.25" customHeight="1">
+    <row r="381" spans="7:7" ht="14.25" customHeight="1">
       <c r="G381" s="3"/>
     </row>
-    <row r="382" ht="14.25" customHeight="1">
+    <row r="382" spans="7:7" ht="14.25" customHeight="1">
       <c r="G382" s="3"/>
     </row>
-    <row r="383" ht="14.25" customHeight="1">
+    <row r="383" spans="7:7" ht="14.25" customHeight="1">
       <c r="G383" s="3"/>
     </row>
-    <row r="384" ht="14.25" customHeight="1">
+    <row r="384" spans="7:7" ht="14.25" customHeight="1">
       <c r="G384" s="3"/>
     </row>
-    <row r="385" ht="14.25" customHeight="1">
+    <row r="385" spans="7:7" ht="14.25" customHeight="1">
       <c r="G385" s="3"/>
     </row>
-    <row r="386" ht="14.25" customHeight="1">
+    <row r="386" spans="7:7" ht="14.25" customHeight="1">
       <c r="G386" s="3"/>
     </row>
-    <row r="387" ht="14.25" customHeight="1">
+    <row r="387" spans="7:7" ht="14.25" customHeight="1">
       <c r="G387" s="3"/>
     </row>
-    <row r="388" ht="14.25" customHeight="1">
+    <row r="388" spans="7:7" ht="14.25" customHeight="1">
       <c r="G388" s="3"/>
     </row>
-    <row r="389" ht="14.25" customHeight="1">
+    <row r="389" spans="7:7" ht="14.25" customHeight="1">
       <c r="G389" s="3"/>
     </row>
-    <row r="390" ht="14.25" customHeight="1">
+    <row r="390" spans="7:7" ht="14.25" customHeight="1">
       <c r="G390" s="3"/>
     </row>
-    <row r="391" ht="14.25" customHeight="1">
+    <row r="391" spans="7:7" ht="14.25" customHeight="1">
       <c r="G391" s="3"/>
     </row>
-    <row r="392" ht="14.25" customHeight="1">
+    <row r="392" spans="7:7" ht="14.25" customHeight="1">
       <c r="G392" s="3"/>
     </row>
-    <row r="393" ht="14.25" customHeight="1">
+    <row r="393" spans="7:7" ht="14.25" customHeight="1">
       <c r="G393" s="3"/>
     </row>
-    <row r="394" ht="14.25" customHeight="1">
+    <row r="394" spans="7:7" ht="14.25" customHeight="1">
       <c r="G394" s="3"/>
     </row>
-    <row r="395" ht="14.25" customHeight="1">
+    <row r="395" spans="7:7" ht="14.25" customHeight="1">
       <c r="G395" s="3"/>
     </row>
-    <row r="396" ht="14.25" customHeight="1">
+    <row r="396" spans="7:7" ht="14.25" customHeight="1">
       <c r="G396" s="3"/>
     </row>
-    <row r="397" ht="14.25" customHeight="1">
+    <row r="397" spans="7:7" ht="14.25" customHeight="1">
       <c r="G397" s="3"/>
     </row>
-    <row r="398" ht="14.25" customHeight="1">
+    <row r="398" spans="7:7" ht="14.25" customHeight="1">
       <c r="G398" s="3"/>
     </row>
-    <row r="399" ht="14.25" customHeight="1">
+    <row r="399" spans="7:7" ht="14.25" customHeight="1">
       <c r="G399" s="3"/>
     </row>
-    <row r="400" ht="14.25" customHeight="1">
+    <row r="400" spans="7:7" ht="14.25" customHeight="1">
       <c r="G400" s="3"/>
     </row>
-    <row r="401" ht="14.25" customHeight="1">
+    <row r="401" spans="7:7" ht="14.25" customHeight="1">
       <c r="G401" s="3"/>
     </row>
-    <row r="402" ht="14.25" customHeight="1">
+    <row r="402" spans="7:7" ht="14.25" customHeight="1">
       <c r="G402" s="3"/>
     </row>
-    <row r="403" ht="14.25" customHeight="1">
+    <row r="403" spans="7:7" ht="14.25" customHeight="1">
       <c r="G403" s="3"/>
     </row>
-    <row r="404" ht="14.25" customHeight="1">
+    <row r="404" spans="7:7" ht="14.25" customHeight="1">
       <c r="G404" s="3"/>
     </row>
-    <row r="405" ht="14.25" customHeight="1">
+    <row r="405" spans="7:7" ht="14.25" customHeight="1">
       <c r="G405" s="3"/>
     </row>
-    <row r="406" ht="14.25" customHeight="1">
+    <row r="406" spans="7:7" ht="14.25" customHeight="1">
       <c r="G406" s="3"/>
     </row>
-    <row r="407" ht="14.25" customHeight="1">
+    <row r="407" spans="7:7" ht="14.25" customHeight="1">
       <c r="G407" s="3"/>
     </row>
-    <row r="408" ht="14.25" customHeight="1">
+    <row r="408" spans="7:7" ht="14.25" customHeight="1">
       <c r="G408" s="3"/>
     </row>
-    <row r="409" ht="14.25" customHeight="1">
+    <row r="409" spans="7:7" ht="14.25" customHeight="1">
       <c r="G409" s="3"/>
     </row>
-    <row r="410" ht="14.25" customHeight="1">
+    <row r="410" spans="7:7" ht="14.25" customHeight="1">
       <c r="G410" s="3"/>
     </row>
-    <row r="411" ht="14.25" customHeight="1">
+    <row r="411" spans="7:7" ht="14.25" customHeight="1">
       <c r="G411" s="3"/>
     </row>
-    <row r="412" ht="14.25" customHeight="1">
+    <row r="412" spans="7:7" ht="14.25" customHeight="1">
       <c r="G412" s="3"/>
     </row>
-    <row r="413" ht="14.25" customHeight="1">
+    <row r="413" spans="7:7" ht="14.25" customHeight="1">
       <c r="G413" s="3"/>
     </row>
-    <row r="414" ht="14.25" customHeight="1">
+    <row r="414" spans="7:7" ht="14.25" customHeight="1">
       <c r="G414" s="3"/>
     </row>
-    <row r="415" ht="14.25" customHeight="1">
+    <row r="415" spans="7:7" ht="14.25" customHeight="1">
       <c r="G415" s="3"/>
     </row>
-    <row r="416" ht="14.25" customHeight="1">
+    <row r="416" spans="7:7" ht="14.25" customHeight="1">
       <c r="G416" s="3"/>
     </row>
-    <row r="417" ht="14.25" customHeight="1">
+    <row r="417" spans="7:7" ht="14.25" customHeight="1">
       <c r="G417" s="3"/>
     </row>
-    <row r="418" ht="14.25" customHeight="1">
+    <row r="418" spans="7:7" ht="14.25" customHeight="1">
       <c r="G418" s="3"/>
     </row>
-    <row r="419" ht="14.25" customHeight="1">
+    <row r="419" spans="7:7" ht="14.25" customHeight="1">
       <c r="G419" s="3"/>
     </row>
-    <row r="420" ht="14.25" customHeight="1">
+    <row r="420" spans="7:7" ht="14.25" customHeight="1">
       <c r="G420" s="3"/>
     </row>
-    <row r="421" ht="14.25" customHeight="1">
+    <row r="421" spans="7:7" ht="14.25" customHeight="1">
       <c r="G421" s="3"/>
     </row>
-    <row r="422" ht="14.25" customHeight="1">
+    <row r="422" spans="7:7" ht="14.25" customHeight="1">
       <c r="G422" s="3"/>
     </row>
-    <row r="423" ht="14.25" customHeight="1">
+    <row r="423" spans="7:7" ht="14.25" customHeight="1">
       <c r="G423" s="3"/>
     </row>
-    <row r="424" ht="14.25" customHeight="1">
+    <row r="424" spans="7:7" ht="14.25" customHeight="1">
       <c r="G424" s="3"/>
     </row>
-    <row r="425" ht="14.25" customHeight="1">
+    <row r="425" spans="7:7" ht="14.25" customHeight="1">
       <c r="G425" s="3"/>
     </row>
-    <row r="426" ht="14.25" customHeight="1">
+    <row r="426" spans="7:7" ht="14.25" customHeight="1">
       <c r="G426" s="3"/>
     </row>
-    <row r="427" ht="14.25" customHeight="1">
+    <row r="427" spans="7:7" ht="14.25" customHeight="1">
       <c r="G427" s="3"/>
     </row>
-    <row r="428" ht="14.25" customHeight="1">
+    <row r="428" spans="7:7" ht="14.25" customHeight="1">
       <c r="G428" s="3"/>
     </row>
-    <row r="429" ht="14.25" customHeight="1">
+    <row r="429" spans="7:7" ht="14.25" customHeight="1">
       <c r="G429" s="3"/>
     </row>
-    <row r="430" ht="14.25" customHeight="1">
+    <row r="430" spans="7:7" ht="14.25" customHeight="1">
       <c r="G430" s="3"/>
     </row>
-    <row r="431" ht="14.25" customHeight="1">
+    <row r="431" spans="7:7" ht="14.25" customHeight="1">
       <c r="G431" s="3"/>
     </row>
-    <row r="432" ht="14.25" customHeight="1">
+    <row r="432" spans="7:7" ht="14.25" customHeight="1">
       <c r="G432" s="3"/>
     </row>
-    <row r="433" ht="14.25" customHeight="1">
+    <row r="433" spans="7:7" ht="14.25" customHeight="1">
       <c r="G433" s="3"/>
     </row>
-    <row r="434" ht="14.25" customHeight="1">
+    <row r="434" spans="7:7" ht="14.25" customHeight="1">
       <c r="G434" s="3"/>
     </row>
-    <row r="435" ht="14.25" customHeight="1">
+    <row r="435" spans="7:7" ht="14.25" customHeight="1">
       <c r="G435" s="3"/>
     </row>
-    <row r="436" ht="14.25" customHeight="1">
+    <row r="436" spans="7:7" ht="14.25" customHeight="1">
       <c r="G436" s="3"/>
     </row>
-    <row r="437" ht="14.25" customHeight="1">
+    <row r="437" spans="7:7" ht="14.25" customHeight="1">
       <c r="G437" s="3"/>
     </row>
-    <row r="438" ht="14.25" customHeight="1">
+    <row r="438" spans="7:7" ht="14.25" customHeight="1">
       <c r="G438" s="3"/>
     </row>
-    <row r="439" ht="14.25" customHeight="1">
+    <row r="439" spans="7:7" ht="14.25" customHeight="1">
       <c r="G439" s="3"/>
     </row>
-    <row r="440" ht="14.25" customHeight="1">
+    <row r="440" spans="7:7" ht="14.25" customHeight="1">
       <c r="G440" s="3"/>
     </row>
-    <row r="441" ht="14.25" customHeight="1">
+    <row r="441" spans="7:7" ht="14.25" customHeight="1">
       <c r="G441" s="3"/>
     </row>
-    <row r="442" ht="14.25" customHeight="1">
+    <row r="442" spans="7:7" ht="14.25" customHeight="1">
       <c r="G442" s="3"/>
     </row>
-    <row r="443" ht="14.25" customHeight="1">
+    <row r="443" spans="7:7" ht="14.25" customHeight="1">
       <c r="G443" s="3"/>
     </row>
-    <row r="444" ht="14.25" customHeight="1">
+    <row r="444" spans="7:7" ht="14.25" customHeight="1">
       <c r="G444" s="3"/>
     </row>
-    <row r="445" ht="14.25" customHeight="1">
+    <row r="445" spans="7:7" ht="14.25" customHeight="1">
       <c r="G445" s="3"/>
     </row>
-    <row r="446" ht="14.25" customHeight="1">
+    <row r="446" spans="7:7" ht="14.25" customHeight="1">
       <c r="G446" s="3"/>
     </row>
-    <row r="447" ht="14.25" customHeight="1">
+    <row r="447" spans="7:7" ht="14.25" customHeight="1">
       <c r="G447" s="3"/>
     </row>
-    <row r="448" ht="14.25" customHeight="1">
+    <row r="448" spans="7:7" ht="14.25" customHeight="1">
       <c r="G448" s="3"/>
     </row>
-    <row r="449" ht="14.25" customHeight="1">
+    <row r="449" spans="7:7" ht="14.25" customHeight="1">
       <c r="G449" s="3"/>
     </row>
-    <row r="450" ht="14.25" customHeight="1">
+    <row r="450" spans="7:7" ht="14.25" customHeight="1">
       <c r="G450" s="3"/>
     </row>
-    <row r="451" ht="14.25" customHeight="1">
+    <row r="451" spans="7:7" ht="14.25" customHeight="1">
       <c r="G451" s="3"/>
     </row>
-    <row r="452" ht="14.25" customHeight="1">
+    <row r="452" spans="7:7" ht="14.25" customHeight="1">
       <c r="G452" s="3"/>
     </row>
-    <row r="453" ht="14.25" customHeight="1">
+    <row r="453" spans="7:7" ht="14.25" customHeight="1">
       <c r="G453" s="3"/>
     </row>
-    <row r="454" ht="14.25" customHeight="1">
+    <row r="454" spans="7:7" ht="14.25" customHeight="1">
       <c r="G454" s="3"/>
     </row>
-    <row r="455" ht="14.25" customHeight="1">
+    <row r="455" spans="7:7" ht="14.25" customHeight="1">
       <c r="G455" s="3"/>
     </row>
-    <row r="456" ht="14.25" customHeight="1">
+    <row r="456" spans="7:7" ht="14.25" customHeight="1">
       <c r="G456" s="3"/>
     </row>
-    <row r="457" ht="14.25" customHeight="1">
+    <row r="457" spans="7:7" ht="14.25" customHeight="1">
       <c r="G457" s="3"/>
     </row>
-    <row r="458" ht="14.25" customHeight="1">
+    <row r="458" spans="7:7" ht="14.25" customHeight="1">
       <c r="G458" s="3"/>
     </row>
-    <row r="459" ht="14.25" customHeight="1">
+    <row r="459" spans="7:7" ht="14.25" customHeight="1">
       <c r="G459" s="3"/>
     </row>
-    <row r="460" ht="14.25" customHeight="1">
+    <row r="460" spans="7:7" ht="14.25" customHeight="1">
       <c r="G460" s="3"/>
     </row>
-    <row r="461" ht="14.25" customHeight="1">
+    <row r="461" spans="7:7" ht="14.25" customHeight="1">
       <c r="G461" s="3"/>
     </row>
-    <row r="462" ht="14.25" customHeight="1">
+    <row r="462" spans="7:7" ht="14.25" customHeight="1">
       <c r="G462" s="3"/>
     </row>
-    <row r="463" ht="14.25" customHeight="1">
+    <row r="463" spans="7:7" ht="14.25" customHeight="1">
       <c r="G463" s="3"/>
     </row>
-    <row r="464" ht="14.25" customHeight="1">
+    <row r="464" spans="7:7" ht="14.25" customHeight="1">
       <c r="G464" s="3"/>
     </row>
-    <row r="465" ht="14.25" customHeight="1">
+    <row r="465" spans="7:7" ht="14.25" customHeight="1">
       <c r="G465" s="3"/>
     </row>
-    <row r="466" ht="14.25" customHeight="1">
+    <row r="466" spans="7:7" ht="14.25" customHeight="1">
       <c r="G466" s="3"/>
     </row>
-    <row r="467" ht="14.25" customHeight="1">
+    <row r="467" spans="7:7" ht="14.25" customHeight="1">
       <c r="G467" s="3"/>
     </row>
-    <row r="468" ht="14.25" customHeight="1">
+    <row r="468" spans="7:7" ht="14.25" customHeight="1">
       <c r="G468" s="3"/>
     </row>
-    <row r="469" ht="14.25" customHeight="1">
+    <row r="469" spans="7:7" ht="14.25" customHeight="1">
       <c r="G469" s="3"/>
     </row>
-    <row r="470" ht="14.25" customHeight="1">
+    <row r="470" spans="7:7" ht="14.25" customHeight="1">
       <c r="G470" s="3"/>
     </row>
-    <row r="471" ht="14.25" customHeight="1">
+    <row r="471" spans="7:7" ht="14.25" customHeight="1">
       <c r="G471" s="3"/>
     </row>
-    <row r="472" ht="14.25" customHeight="1">
+    <row r="472" spans="7:7" ht="14.25" customHeight="1">
       <c r="G472" s="3"/>
     </row>
-    <row r="473" ht="14.25" customHeight="1">
+    <row r="473" spans="7:7" ht="14.25" customHeight="1">
       <c r="G473" s="3"/>
     </row>
-    <row r="474" ht="14.25" customHeight="1">
+    <row r="474" spans="7:7" ht="14.25" customHeight="1">
       <c r="G474" s="3"/>
     </row>
-    <row r="475" ht="14.25" customHeight="1">
+    <row r="475" spans="7:7" ht="14.25" customHeight="1">
       <c r="G475" s="3"/>
     </row>
-    <row r="476" ht="14.25" customHeight="1">
+    <row r="476" spans="7:7" ht="14.25" customHeight="1">
       <c r="G476" s="3"/>
     </row>
-    <row r="477" ht="14.25" customHeight="1">
+    <row r="477" spans="7:7" ht="14.25" customHeight="1">
       <c r="G477" s="3"/>
     </row>
-    <row r="478" ht="14.25" customHeight="1">
+    <row r="478" spans="7:7" ht="14.25" customHeight="1">
       <c r="G478" s="3"/>
     </row>
-    <row r="479" ht="14.25" customHeight="1">
+    <row r="479" spans="7:7" ht="14.25" customHeight="1">
       <c r="G479" s="3"/>
     </row>
-    <row r="480" ht="14.25" customHeight="1">
+    <row r="480" spans="7:7" ht="14.25" customHeight="1">
       <c r="G480" s="3"/>
     </row>
-    <row r="481" ht="14.25" customHeight="1">
+    <row r="481" spans="7:7" ht="14.25" customHeight="1">
       <c r="G481" s="3"/>
     </row>
-    <row r="482" ht="14.25" customHeight="1">
+    <row r="482" spans="7:7" ht="14.25" customHeight="1">
       <c r="G482" s="3"/>
     </row>
-    <row r="483" ht="14.25" customHeight="1">
+    <row r="483" spans="7:7" ht="14.25" customHeight="1">
       <c r="G483" s="3"/>
     </row>
-    <row r="484" ht="14.25" customHeight="1">
+    <row r="484" spans="7:7" ht="14.25" customHeight="1">
       <c r="G484" s="3"/>
     </row>
-    <row r="485" ht="14.25" customHeight="1">
+    <row r="485" spans="7:7" ht="14.25" customHeight="1">
       <c r="G485" s="3"/>
     </row>
-    <row r="486" ht="14.25" customHeight="1">
+    <row r="486" spans="7:7" ht="14.25" customHeight="1">
       <c r="G486" s="3"/>
     </row>
-    <row r="487" ht="14.25" customHeight="1">
+    <row r="487" spans="7:7" ht="14.25" customHeight="1">
       <c r="G487" s="3"/>
     </row>
-    <row r="488" ht="14.25" customHeight="1">
+    <row r="488" spans="7:7" ht="14.25" customHeight="1">
       <c r="G488" s="3"/>
     </row>
-    <row r="489" ht="14.25" customHeight="1">
+    <row r="489" spans="7:7" ht="14.25" customHeight="1">
       <c r="G489" s="3"/>
     </row>
-    <row r="490" ht="14.25" customHeight="1">
+    <row r="490" spans="7:7" ht="14.25" customHeight="1">
       <c r="G490" s="3"/>
     </row>
-    <row r="491" ht="14.25" customHeight="1">
+    <row r="491" spans="7:7" ht="14.25" customHeight="1">
       <c r="G491" s="3"/>
     </row>
-    <row r="492" ht="14.25" customHeight="1">
+    <row r="492" spans="7:7" ht="14.25" customHeight="1">
       <c r="G492" s="3"/>
     </row>
-    <row r="493" ht="14.25" customHeight="1">
+    <row r="493" spans="7:7" ht="14.25" customHeight="1">
       <c r="G493" s="3"/>
     </row>
-    <row r="494" ht="14.25" customHeight="1">
+    <row r="494" spans="7:7" ht="14.25" customHeight="1">
       <c r="G494" s="3"/>
     </row>
-    <row r="495" ht="14.25" customHeight="1">
+    <row r="495" spans="7:7" ht="14.25" customHeight="1">
       <c r="G495" s="3"/>
     </row>
-    <row r="496" ht="14.25" customHeight="1">
+    <row r="496" spans="7:7" ht="14.25" customHeight="1">
       <c r="G496" s="3"/>
     </row>
-    <row r="497" ht="14.25" customHeight="1">
+    <row r="497" spans="7:7" ht="14.25" customHeight="1">
       <c r="G497" s="3"/>
     </row>
-    <row r="498" ht="14.25" customHeight="1">
+    <row r="498" spans="7:7" ht="14.25" customHeight="1">
       <c r="G498" s="3"/>
     </row>
-    <row r="499" ht="14.25" customHeight="1">
+    <row r="499" spans="7:7" ht="14.25" customHeight="1">
       <c r="G499" s="3"/>
     </row>
-    <row r="500" ht="14.25" customHeight="1">
+    <row r="500" spans="7:7" ht="14.25" customHeight="1">
       <c r="G500" s="3"/>
     </row>
-    <row r="501" ht="14.25" customHeight="1">
+    <row r="501" spans="7:7" ht="14.25" customHeight="1">
       <c r="G501" s="3"/>
     </row>
-    <row r="502" ht="14.25" customHeight="1">
+    <row r="502" spans="7:7" ht="14.25" customHeight="1">
       <c r="G502" s="3"/>
     </row>
-    <row r="503" ht="14.25" customHeight="1">
+    <row r="503" spans="7:7" ht="14.25" customHeight="1">
       <c r="G503" s="3"/>
     </row>
-    <row r="504" ht="14.25" customHeight="1">
+    <row r="504" spans="7:7" ht="14.25" customHeight="1">
       <c r="G504" s="3"/>
     </row>
-    <row r="505" ht="14.25" customHeight="1">
+    <row r="505" spans="7:7" ht="14.25" customHeight="1">
       <c r="G505" s="3"/>
     </row>
-    <row r="506" ht="14.25" customHeight="1">
+    <row r="506" spans="7:7" ht="14.25" customHeight="1">
       <c r="G506" s="3"/>
     </row>
-    <row r="507" ht="14.25" customHeight="1">
+    <row r="507" spans="7:7" ht="14.25" customHeight="1">
       <c r="G507" s="3"/>
     </row>
-    <row r="508" ht="14.25" customHeight="1">
+    <row r="508" spans="7:7" ht="14.25" customHeight="1">
       <c r="G508" s="3"/>
     </row>
-    <row r="509" ht="14.25" customHeight="1">
+    <row r="509" spans="7:7" ht="14.25" customHeight="1">
       <c r="G509" s="3"/>
     </row>
-    <row r="510" ht="14.25" customHeight="1">
+    <row r="510" spans="7:7" ht="14.25" customHeight="1">
       <c r="G510" s="3"/>
     </row>
-    <row r="511" ht="14.25" customHeight="1">
+    <row r="511" spans="7:7" ht="14.25" customHeight="1">
       <c r="G511" s="3"/>
     </row>
-    <row r="512" ht="14.25" customHeight="1">
+    <row r="512" spans="7:7" ht="14.25" customHeight="1">
       <c r="G512" s="3"/>
     </row>
-    <row r="513" ht="14.25" customHeight="1">
+    <row r="513" spans="7:7" ht="14.25" customHeight="1">
       <c r="G513" s="3"/>
     </row>
-    <row r="514" ht="14.25" customHeight="1">
+    <row r="514" spans="7:7" ht="14.25" customHeight="1">
       <c r="G514" s="3"/>
     </row>
-    <row r="515" ht="14.25" customHeight="1">
+    <row r="515" spans="7:7" ht="14.25" customHeight="1">
       <c r="G515" s="3"/>
     </row>
-    <row r="516" ht="14.25" customHeight="1">
+    <row r="516" spans="7:7" ht="14.25" customHeight="1">
       <c r="G516" s="3"/>
     </row>
-    <row r="517" ht="14.25" customHeight="1">
+    <row r="517" spans="7:7" ht="14.25" customHeight="1">
       <c r="G517" s="3"/>
     </row>
-    <row r="518" ht="14.25" customHeight="1">
+    <row r="518" spans="7:7" ht="14.25" customHeight="1">
       <c r="G518" s="3"/>
     </row>
-    <row r="519" ht="14.25" customHeight="1">
+    <row r="519" spans="7:7" ht="14.25" customHeight="1">
       <c r="G519" s="3"/>
     </row>
-    <row r="520" ht="14.25" customHeight="1">
+    <row r="520" spans="7:7" ht="14.25" customHeight="1">
       <c r="G520" s="3"/>
     </row>
-    <row r="521" ht="14.25" customHeight="1">
+    <row r="521" spans="7:7" ht="14.25" customHeight="1">
       <c r="G521" s="3"/>
     </row>
-    <row r="522" ht="14.25" customHeight="1">
+    <row r="522" spans="7:7" ht="14.25" customHeight="1">
       <c r="G522" s="3"/>
     </row>
-    <row r="523" ht="14.25" customHeight="1">
+    <row r="523" spans="7:7" ht="14.25" customHeight="1">
       <c r="G523" s="3"/>
     </row>
-    <row r="524" ht="14.25" customHeight="1">
+    <row r="524" spans="7:7" ht="14.25" customHeight="1">
       <c r="G524" s="3"/>
     </row>
-    <row r="525" ht="14.25" customHeight="1">
+    <row r="525" spans="7:7" ht="14.25" customHeight="1">
       <c r="G525" s="3"/>
     </row>
-    <row r="526" ht="14.25" customHeight="1">
+    <row r="526" spans="7:7" ht="14.25" customHeight="1">
       <c r="G526" s="3"/>
     </row>
-    <row r="527" ht="14.25" customHeight="1">
+    <row r="527" spans="7:7" ht="14.25" customHeight="1">
       <c r="G527" s="3"/>
     </row>
-    <row r="528" ht="14.25" customHeight="1">
+    <row r="528" spans="7:7" ht="14.25" customHeight="1">
       <c r="G528" s="3"/>
     </row>
-    <row r="529" ht="14.25" customHeight="1">
+    <row r="529" spans="7:7" ht="14.25" customHeight="1">
       <c r="G529" s="3"/>
     </row>
-    <row r="530" ht="14.25" customHeight="1">
+    <row r="530" spans="7:7" ht="14.25" customHeight="1">
       <c r="G530" s="3"/>
     </row>
-    <row r="531" ht="14.25" customHeight="1">
+    <row r="531" spans="7:7" ht="14.25" customHeight="1">
       <c r="G531" s="3"/>
     </row>
-    <row r="532" ht="14.25" customHeight="1">
+    <row r="532" spans="7:7" ht="14.25" customHeight="1">
       <c r="G532" s="3"/>
     </row>
-    <row r="533" ht="14.25" customHeight="1">
+    <row r="533" spans="7:7" ht="14.25" customHeight="1">
       <c r="G533" s="3"/>
     </row>
-    <row r="534" ht="14.25" customHeight="1">
+    <row r="534" spans="7:7" ht="14.25" customHeight="1">
       <c r="G534" s="3"/>
     </row>
-    <row r="535" ht="14.25" customHeight="1">
+    <row r="535" spans="7:7" ht="14.25" customHeight="1">
       <c r="G535" s="3"/>
     </row>
-    <row r="536" ht="14.25" customHeight="1">
+    <row r="536" spans="7:7" ht="14.25" customHeight="1">
       <c r="G536" s="3"/>
     </row>
-    <row r="537" ht="14.25" customHeight="1">
+    <row r="537" spans="7:7" ht="14.25" customHeight="1">
       <c r="G537" s="3"/>
     </row>
-    <row r="538" ht="14.25" customHeight="1">
+    <row r="538" spans="7:7" ht="14.25" customHeight="1">
       <c r="G538" s="3"/>
     </row>
-    <row r="539" ht="14.25" customHeight="1">
+    <row r="539" spans="7:7" ht="14.25" customHeight="1">
       <c r="G539" s="3"/>
     </row>
-    <row r="540" ht="14.25" customHeight="1">
+    <row r="540" spans="7:7" ht="14.25" customHeight="1">
       <c r="G540" s="3"/>
     </row>
-    <row r="541" ht="14.25" customHeight="1">
+    <row r="541" spans="7:7" ht="14.25" customHeight="1">
       <c r="G541" s="3"/>
     </row>
-    <row r="542" ht="14.25" customHeight="1">
+    <row r="542" spans="7:7" ht="14.25" customHeight="1">
       <c r="G542" s="3"/>
     </row>
-    <row r="543" ht="14.25" customHeight="1">
+    <row r="543" spans="7:7" ht="14.25" customHeight="1">
       <c r="G543" s="3"/>
     </row>
-    <row r="544" ht="14.25" customHeight="1">
+    <row r="544" spans="7:7" ht="14.25" customHeight="1">
       <c r="G544" s="3"/>
     </row>
-    <row r="545" ht="14.25" customHeight="1">
+    <row r="545" spans="7:7" ht="14.25" customHeight="1">
       <c r="G545" s="3"/>
     </row>
-    <row r="546" ht="14.25" customHeight="1">
+    <row r="546" spans="7:7" ht="14.25" customHeight="1">
       <c r="G546" s="3"/>
     </row>
-    <row r="547" ht="14.25" customHeight="1">
+    <row r="547" spans="7:7" ht="14.25" customHeight="1">
       <c r="G547" s="3"/>
     </row>
-    <row r="548" ht="14.25" customHeight="1">
+    <row r="548" spans="7:7" ht="14.25" customHeight="1">
       <c r="G548" s="3"/>
     </row>
-    <row r="549" ht="14.25" customHeight="1">
+    <row r="549" spans="7:7" ht="14.25" customHeight="1">
       <c r="G549" s="3"/>
     </row>
-    <row r="550" ht="14.25" customHeight="1">
+    <row r="550" spans="7:7" ht="14.25" customHeight="1">
       <c r="G550" s="3"/>
     </row>
-    <row r="551" ht="14.25" customHeight="1">
+    <row r="551" spans="7:7" ht="14.25" customHeight="1">
       <c r="G551" s="3"/>
     </row>
-    <row r="552" ht="14.25" customHeight="1">
+    <row r="552" spans="7:7" ht="14.25" customHeight="1">
       <c r="G552" s="3"/>
     </row>
-    <row r="553" ht="14.25" customHeight="1">
+    <row r="553" spans="7:7" ht="14.25" customHeight="1">
       <c r="G553" s="3"/>
     </row>
-    <row r="554" ht="14.25" customHeight="1">
+    <row r="554" spans="7:7" ht="14.25" customHeight="1">
       <c r="G554" s="3"/>
     </row>
-    <row r="555" ht="14.25" customHeight="1">
+    <row r="555" spans="7:7" ht="14.25" customHeight="1">
       <c r="G555" s="3"/>
     </row>
-    <row r="556" ht="14.25" customHeight="1">
+    <row r="556" spans="7:7" ht="14.25" customHeight="1">
       <c r="G556" s="3"/>
     </row>
-    <row r="557" ht="14.25" customHeight="1">
+    <row r="557" spans="7:7" ht="14.25" customHeight="1">
       <c r="G557" s="3"/>
     </row>
-    <row r="558" ht="14.25" customHeight="1">
+    <row r="558" spans="7:7" ht="14.25" customHeight="1">
       <c r="G558" s="3"/>
     </row>
-    <row r="559" ht="14.25" customHeight="1">
+    <row r="559" spans="7:7" ht="14.25" customHeight="1">
       <c r="G559" s="3"/>
     </row>
-    <row r="560" ht="14.25" customHeight="1">
+    <row r="560" spans="7:7" ht="14.25" customHeight="1">
       <c r="G560" s="3"/>
     </row>
-    <row r="561" ht="14.25" customHeight="1">
+    <row r="561" spans="7:7" ht="14.25" customHeight="1">
       <c r="G561" s="3"/>
     </row>
-    <row r="562" ht="14.25" customHeight="1">
+    <row r="562" spans="7:7" ht="14.25" customHeight="1">
       <c r="G562" s="3"/>
     </row>
-    <row r="563" ht="14.25" customHeight="1">
+    <row r="563" spans="7:7" ht="14.25" customHeight="1">
       <c r="G563" s="3"/>
     </row>
-    <row r="564" ht="14.25" customHeight="1">
+    <row r="564" spans="7:7" ht="14.25" customHeight="1">
       <c r="G564" s="3"/>
     </row>
-    <row r="565" ht="14.25" customHeight="1">
+    <row r="565" spans="7:7" ht="14.25" customHeight="1">
       <c r="G565" s="3"/>
     </row>
-    <row r="566" ht="14.25" customHeight="1">
+    <row r="566" spans="7:7" ht="14.25" customHeight="1">
       <c r="G566" s="3"/>
     </row>
-    <row r="567" ht="14.25" customHeight="1">
+    <row r="567" spans="7:7" ht="14.25" customHeight="1">
       <c r="G567" s="3"/>
     </row>
-    <row r="568" ht="14.25" customHeight="1">
+    <row r="568" spans="7:7" ht="14.25" customHeight="1">
       <c r="G568" s="3"/>
     </row>
-    <row r="569" ht="14.25" customHeight="1">
+    <row r="569" spans="7:7" ht="14.25" customHeight="1">
       <c r="G569" s="3"/>
     </row>
-    <row r="570" ht="14.25" customHeight="1">
+    <row r="570" spans="7:7" ht="14.25" customHeight="1">
       <c r="G570" s="3"/>
     </row>
-    <row r="571" ht="14.25" customHeight="1">
+    <row r="571" spans="7:7" ht="14.25" customHeight="1">
       <c r="G571" s="3"/>
     </row>
-    <row r="572" ht="14.25" customHeight="1">
+    <row r="572" spans="7:7" ht="14.25" customHeight="1">
       <c r="G572" s="3"/>
     </row>
-    <row r="573" ht="14.25" customHeight="1">
+    <row r="573" spans="7:7" ht="14.25" customHeight="1">
       <c r="G573" s="3"/>
     </row>
-    <row r="574" ht="14.25" customHeight="1">
+    <row r="574" spans="7:7" ht="14.25" customHeight="1">
       <c r="G574" s="3"/>
     </row>
-    <row r="575" ht="14.25" customHeight="1">
+    <row r="575" spans="7:7" ht="14.25" customHeight="1">
       <c r="G575" s="3"/>
     </row>
-    <row r="576" ht="14.25" customHeight="1">
+    <row r="576" spans="7:7" ht="14.25" customHeight="1">
       <c r="G576" s="3"/>
     </row>
-    <row r="577" ht="14.25" customHeight="1">
+    <row r="577" spans="7:7" ht="14.25" customHeight="1">
       <c r="G577" s="3"/>
     </row>
-    <row r="578" ht="14.25" customHeight="1">
+    <row r="578" spans="7:7" ht="14.25" customHeight="1">
       <c r="G578" s="3"/>
     </row>
-    <row r="579" ht="14.25" customHeight="1">
+    <row r="579" spans="7:7" ht="14.25" customHeight="1">
       <c r="G579" s="3"/>
     </row>
-    <row r="580" ht="14.25" customHeight="1">
+    <row r="580" spans="7:7" ht="14.25" customHeight="1">
       <c r="G580" s="3"/>
     </row>
-    <row r="581" ht="14.25" customHeight="1">
+    <row r="581" spans="7:7" ht="14.25" customHeight="1">
       <c r="G581" s="3"/>
     </row>
-    <row r="582" ht="14.25" customHeight="1">
+    <row r="582" spans="7:7" ht="14.25" customHeight="1">
       <c r="G582" s="3"/>
     </row>
-    <row r="583" ht="14.25" customHeight="1">
+    <row r="583" spans="7:7" ht="14.25" customHeight="1">
       <c r="G583" s="3"/>
     </row>
-    <row r="584" ht="14.25" customHeight="1">
+    <row r="584" spans="7:7" ht="14.25" customHeight="1">
       <c r="G584" s="3"/>
     </row>
-    <row r="585" ht="14.25" customHeight="1">
+    <row r="585" spans="7:7" ht="14.25" customHeight="1">
       <c r="G585" s="3"/>
     </row>
-    <row r="586" ht="14.25" customHeight="1">
+    <row r="586" spans="7:7" ht="14.25" customHeight="1">
       <c r="G586" s="3"/>
     </row>
-    <row r="587" ht="14.25" customHeight="1">
+    <row r="587" spans="7:7" ht="14.25" customHeight="1">
       <c r="G587" s="3"/>
     </row>
-    <row r="588" ht="14.25" customHeight="1">
+    <row r="588" spans="7:7" ht="14.25" customHeight="1">
       <c r="G588" s="3"/>
     </row>
-    <row r="589" ht="14.25" customHeight="1">
+    <row r="589" spans="7:7" ht="14.25" customHeight="1">
       <c r="G589" s="3"/>
     </row>
-    <row r="590" ht="14.25" customHeight="1">
+    <row r="590" spans="7:7" ht="14.25" customHeight="1">
       <c r="G590" s="3"/>
     </row>
-    <row r="591" ht="14.25" customHeight="1">
+    <row r="591" spans="7:7" ht="14.25" customHeight="1">
       <c r="G591" s="3"/>
     </row>
-    <row r="592" ht="14.25" customHeight="1">
+    <row r="592" spans="7:7" ht="14.25" customHeight="1">
       <c r="G592" s="3"/>
     </row>
-    <row r="593" ht="14.25" customHeight="1">
+    <row r="593" spans="7:7" ht="14.25" customHeight="1">
       <c r="G593" s="3"/>
     </row>
-    <row r="594" ht="14.25" customHeight="1">
+    <row r="594" spans="7:7" ht="14.25" customHeight="1">
       <c r="G594" s="3"/>
     </row>
-    <row r="595" ht="14.25" customHeight="1">
+    <row r="595" spans="7:7" ht="14.25" customHeight="1">
       <c r="G595" s="3"/>
     </row>
-    <row r="596" ht="14.25" customHeight="1">
+    <row r="596" spans="7:7" ht="14.25" customHeight="1">
       <c r="G596" s="3"/>
     </row>
-    <row r="597" ht="14.25" customHeight="1">
+    <row r="597" spans="7:7" ht="14.25" customHeight="1">
       <c r="G597" s="3"/>
     </row>
-    <row r="598" ht="14.25" customHeight="1">
+    <row r="598" spans="7:7" ht="14.25" customHeight="1">
       <c r="G598" s="3"/>
     </row>
-    <row r="599" ht="14.25" customHeight="1">
+    <row r="599" spans="7:7" ht="14.25" customHeight="1">
       <c r="G599" s="3"/>
     </row>
-    <row r="600" ht="14.25" customHeight="1">
+    <row r="600" spans="7:7" ht="14.25" customHeight="1">
       <c r="G600" s="3"/>
     </row>
-    <row r="601" ht="14.25" customHeight="1">
+    <row r="601" spans="7:7" ht="14.25" customHeight="1">
       <c r="G601" s="3"/>
     </row>
-    <row r="602" ht="14.25" customHeight="1">
+    <row r="602" spans="7:7" ht="14.25" customHeight="1">
       <c r="G602" s="3"/>
     </row>
-    <row r="603" ht="14.25" customHeight="1">
+    <row r="603" spans="7:7" ht="14.25" customHeight="1">
       <c r="G603" s="3"/>
     </row>
-    <row r="604" ht="14.25" customHeight="1">
+    <row r="604" spans="7:7" ht="14.25" customHeight="1">
       <c r="G604" s="3"/>
     </row>
-    <row r="605" ht="14.25" customHeight="1">
+    <row r="605" spans="7:7" ht="14.25" customHeight="1">
       <c r="G605" s="3"/>
     </row>
-    <row r="606" ht="14.25" customHeight="1">
+    <row r="606" spans="7:7" ht="14.25" customHeight="1">
       <c r="G606" s="3"/>
     </row>
-    <row r="607" ht="14.25" customHeight="1">
+    <row r="607" spans="7:7" ht="14.25" customHeight="1">
       <c r="G607" s="3"/>
     </row>
-    <row r="608" ht="14.25" customHeight="1">
+    <row r="608" spans="7:7" ht="14.25" customHeight="1">
       <c r="G608" s="3"/>
     </row>
-    <row r="609" ht="14.25" customHeight="1">
+    <row r="609" spans="7:7" ht="14.25" customHeight="1">
       <c r="G609" s="3"/>
     </row>
-    <row r="610" ht="14.25" customHeight="1">
+    <row r="610" spans="7:7" ht="14.25" customHeight="1">
       <c r="G610" s="3"/>
     </row>
-    <row r="611" ht="14.25" customHeight="1">
+    <row r="611" spans="7:7" ht="14.25" customHeight="1">
       <c r="G611" s="3"/>
     </row>
-    <row r="612" ht="14.25" customHeight="1">
+    <row r="612" spans="7:7" ht="14.25" customHeight="1">
       <c r="G612" s="3"/>
     </row>
-    <row r="613" ht="14.25" customHeight="1">
+    <row r="613" spans="7:7" ht="14.25" customHeight="1">
       <c r="G613" s="3"/>
     </row>
-    <row r="614" ht="14.25" customHeight="1">
+    <row r="614" spans="7:7" ht="14.25" customHeight="1">
       <c r="G614" s="3"/>
     </row>
-    <row r="615" ht="14.25" customHeight="1">
+    <row r="615" spans="7:7" ht="14.25" customHeight="1">
       <c r="G615" s="3"/>
     </row>
-    <row r="616" ht="14.25" customHeight="1">
+    <row r="616" spans="7:7" ht="14.25" customHeight="1">
       <c r="G616" s="3"/>
     </row>
-    <row r="617" ht="14.25" customHeight="1">
+    <row r="617" spans="7:7" ht="14.25" customHeight="1">
       <c r="G617" s="3"/>
     </row>
-    <row r="618" ht="14.25" customHeight="1">
+    <row r="618" spans="7:7" ht="14.25" customHeight="1">
       <c r="G618" s="3"/>
     </row>
-    <row r="619" ht="14.25" customHeight="1">
+    <row r="619" spans="7:7" ht="14.25" customHeight="1">
       <c r="G619" s="3"/>
     </row>
-    <row r="620" ht="14.25" customHeight="1">
+    <row r="620" spans="7:7" ht="14.25" customHeight="1">
       <c r="G620" s="3"/>
     </row>
-    <row r="621" ht="14.25" customHeight="1">
+    <row r="621" spans="7:7" ht="14.25" customHeight="1">
       <c r="G621" s="3"/>
     </row>
-    <row r="622" ht="14.25" customHeight="1">
+    <row r="622" spans="7:7" ht="14.25" customHeight="1">
       <c r="G622" s="3"/>
     </row>
-    <row r="623" ht="14.25" customHeight="1">
+    <row r="623" spans="7:7" ht="14.25" customHeight="1">
       <c r="G623" s="3"/>
     </row>
-    <row r="624" ht="14.25" customHeight="1">
+    <row r="624" spans="7:7" ht="14.25" customHeight="1">
       <c r="G624" s="3"/>
     </row>
-    <row r="625" ht="14.25" customHeight="1">
+    <row r="625" spans="7:7" ht="14.25" customHeight="1">
       <c r="G625" s="3"/>
     </row>
-    <row r="626" ht="14.25" customHeight="1">
+    <row r="626" spans="7:7" ht="14.25" customHeight="1">
       <c r="G626" s="3"/>
     </row>
-    <row r="627" ht="14.25" customHeight="1">
+    <row r="627" spans="7:7" ht="14.25" customHeight="1">
       <c r="G627" s="3"/>
     </row>
-    <row r="628" ht="14.25" customHeight="1">
+    <row r="628" spans="7:7" ht="14.25" customHeight="1">
       <c r="G628" s="3"/>
     </row>
-    <row r="629" ht="14.25" customHeight="1">
+    <row r="629" spans="7:7" ht="14.25" customHeight="1">
       <c r="G629" s="3"/>
     </row>
-    <row r="630" ht="14.25" customHeight="1">
+    <row r="630" spans="7:7" ht="14.25" customHeight="1">
       <c r="G630" s="3"/>
     </row>
-    <row r="631" ht="14.25" customHeight="1">
+    <row r="631" spans="7:7" ht="14.25" customHeight="1">
       <c r="G631" s="3"/>
     </row>
-    <row r="632" ht="14.25" customHeight="1">
+    <row r="632" spans="7:7" ht="14.25" customHeight="1">
       <c r="G632" s="3"/>
     </row>
-    <row r="633" ht="14.25" customHeight="1">
+    <row r="633" spans="7:7" ht="14.25" customHeight="1">
       <c r="G633" s="3"/>
     </row>
-    <row r="634" ht="14.25" customHeight="1">
+    <row r="634" spans="7:7" ht="14.25" customHeight="1">
       <c r="G634" s="3"/>
     </row>
-    <row r="635" ht="14.25" customHeight="1">
+    <row r="635" spans="7:7" ht="14.25" customHeight="1">
       <c r="G635" s="3"/>
     </row>
-    <row r="636" ht="14.25" customHeight="1">
+    <row r="636" spans="7:7" ht="14.25" customHeight="1">
       <c r="G636" s="3"/>
     </row>
-    <row r="637" ht="14.25" customHeight="1">
+    <row r="637" spans="7:7" ht="14.25" customHeight="1">
       <c r="G637" s="3"/>
     </row>
-    <row r="638" ht="14.25" customHeight="1">
+    <row r="638" spans="7:7" ht="14.25" customHeight="1">
       <c r="G638" s="3"/>
     </row>
-    <row r="639" ht="14.25" customHeight="1">
+    <row r="639" spans="7:7" ht="14.25" customHeight="1">
       <c r="G639" s="3"/>
     </row>
-    <row r="640" ht="14.25" customHeight="1">
+    <row r="640" spans="7:7" ht="14.25" customHeight="1">
       <c r="G640" s="3"/>
     </row>
-    <row r="641" ht="14.25" customHeight="1">
+    <row r="641" spans="7:7" ht="14.25" customHeight="1">
       <c r="G641" s="3"/>
     </row>
-    <row r="642" ht="14.25" customHeight="1">
+    <row r="642" spans="7:7" ht="14.25" customHeight="1">
       <c r="G642" s="3"/>
     </row>
-    <row r="643" ht="14.25" customHeight="1">
+    <row r="643" spans="7:7" ht="14.25" customHeight="1">
       <c r="G643" s="3"/>
     </row>
-    <row r="644" ht="14.25" customHeight="1">
+    <row r="644" spans="7:7" ht="14.25" customHeight="1">
       <c r="G644" s="3"/>
     </row>
-    <row r="645" ht="14.25" customHeight="1">
+    <row r="645" spans="7:7" ht="14.25" customHeight="1">
       <c r="G645" s="3"/>
     </row>
-    <row r="646" ht="14.25" customHeight="1">
+    <row r="646" spans="7:7" ht="14.25" customHeight="1">
       <c r="G646" s="3"/>
     </row>
-    <row r="647" ht="14.25" customHeight="1">
+    <row r="647" spans="7:7" ht="14.25" customHeight="1">
       <c r="G647" s="3"/>
     </row>
-    <row r="648" ht="14.25" customHeight="1">
+    <row r="648" spans="7:7" ht="14.25" customHeight="1">
       <c r="G648" s="3"/>
     </row>
-    <row r="649" ht="14.25" customHeight="1">
+    <row r="649" spans="7:7" ht="14.25" customHeight="1">
       <c r="G649" s="3"/>
     </row>
-    <row r="650" ht="14.25" customHeight="1">
+    <row r="650" spans="7:7" ht="14.25" customHeight="1">
       <c r="G650" s="3"/>
     </row>
-    <row r="651" ht="14.25" customHeight="1">
+    <row r="651" spans="7:7" ht="14.25" customHeight="1">
       <c r="G651" s="3"/>
     </row>
-    <row r="652" ht="14.25" customHeight="1">
+    <row r="652" spans="7:7" ht="14.25" customHeight="1">
       <c r="G652" s="3"/>
     </row>
-    <row r="653" ht="14.25" customHeight="1">
+    <row r="653" spans="7:7" ht="14.25" customHeight="1">
       <c r="G653" s="3"/>
     </row>
-    <row r="654" ht="14.25" customHeight="1">
+    <row r="654" spans="7:7" ht="14.25" customHeight="1">
       <c r="G654" s="3"/>
     </row>
-    <row r="655" ht="14.25" customHeight="1">
+    <row r="655" spans="7:7" ht="14.25" customHeight="1">
       <c r="G655" s="3"/>
     </row>
-    <row r="656" ht="14.25" customHeight="1">
+    <row r="656" spans="7:7" ht="14.25" customHeight="1">
       <c r="G656" s="3"/>
     </row>
-    <row r="657" ht="14.25" customHeight="1">
+    <row r="657" spans="7:7" ht="14.25" customHeight="1">
       <c r="G657" s="3"/>
     </row>
-    <row r="658" ht="14.25" customHeight="1">
+    <row r="658" spans="7:7" ht="14.25" customHeight="1">
       <c r="G658" s="3"/>
     </row>
-    <row r="659" ht="14.25" customHeight="1">
+    <row r="659" spans="7:7" ht="14.25" customHeight="1">
       <c r="G659" s="3"/>
     </row>
-    <row r="660" ht="14.25" customHeight="1">
+    <row r="660" spans="7:7" ht="14.25" customHeight="1">
       <c r="G660" s="3"/>
     </row>
-    <row r="661" ht="14.25" customHeight="1">
+    <row r="661" spans="7:7" ht="14.25" customHeight="1">
       <c r="G661" s="3"/>
     </row>
-    <row r="662" ht="14.25" customHeight="1">
+    <row r="662" spans="7:7" ht="14.25" customHeight="1">
       <c r="G662" s="3"/>
     </row>
-    <row r="663" ht="14.25" customHeight="1">
+    <row r="663" spans="7:7" ht="14.25" customHeight="1">
       <c r="G663" s="3"/>
     </row>
-    <row r="664" ht="14.25" customHeight="1">
+    <row r="664" spans="7:7" ht="14.25" customHeight="1">
       <c r="G664" s="3"/>
     </row>
-    <row r="665" ht="14.25" customHeight="1">
+    <row r="665" spans="7:7" ht="14.25" customHeight="1">
       <c r="G665" s="3"/>
     </row>
-    <row r="666" ht="14.25" customHeight="1">
+    <row r="666" spans="7:7" ht="14.25" customHeight="1">
       <c r="G666" s="3"/>
     </row>
-    <row r="667" ht="14.25" customHeight="1">
+    <row r="667" spans="7:7" ht="14.25" customHeight="1">
       <c r="G667" s="3"/>
     </row>
-    <row r="668" ht="14.25" customHeight="1">
+    <row r="668" spans="7:7" ht="14.25" customHeight="1">
       <c r="G668" s="3"/>
     </row>
-    <row r="669" ht="14.25" customHeight="1">
+    <row r="669" spans="7:7" ht="14.25" customHeight="1">
       <c r="G669" s="3"/>
     </row>
-    <row r="670" ht="14.25" customHeight="1">
+    <row r="670" spans="7:7" ht="14.25" customHeight="1">
       <c r="G670" s="3"/>
     </row>
-    <row r="671" ht="14.25" customHeight="1">
+    <row r="671" spans="7:7" ht="14.25" customHeight="1">
       <c r="G671" s="3"/>
     </row>
-    <row r="672" ht="14.25" customHeight="1">
+    <row r="672" spans="7:7" ht="14.25" customHeight="1">
       <c r="G672" s="3"/>
     </row>
-    <row r="673" ht="14.25" customHeight="1">
+    <row r="673" spans="7:7" ht="14.25" customHeight="1">
       <c r="G673" s="3"/>
     </row>
-    <row r="674" ht="14.25" customHeight="1">
+    <row r="674" spans="7:7" ht="14.25" customHeight="1">
       <c r="G674" s="3"/>
     </row>
-    <row r="675" ht="14.25" customHeight="1">
+    <row r="675" spans="7:7" ht="14.25" customHeight="1">
       <c r="G675" s="3"/>
     </row>
-    <row r="676" ht="14.25" customHeight="1">
+    <row r="676" spans="7:7" ht="14.25" customHeight="1">
       <c r="G676" s="3"/>
     </row>
-    <row r="677" ht="14.25" customHeight="1">
+    <row r="677" spans="7:7" ht="14.25" customHeight="1">
       <c r="G677" s="3"/>
     </row>
-    <row r="678" ht="14.25" customHeight="1">
+    <row r="678" spans="7:7" ht="14.25" customHeight="1">
       <c r="G678" s="3"/>
     </row>
-    <row r="679" ht="14.25" customHeight="1">
+    <row r="679" spans="7:7" ht="14.25" customHeight="1">
       <c r="G679" s="3"/>
     </row>
-    <row r="680" ht="14.25" customHeight="1">
+    <row r="680" spans="7:7" ht="14.25" customHeight="1">
       <c r="G680" s="3"/>
     </row>
-    <row r="681" ht="14.25" customHeight="1">
+    <row r="681" spans="7:7" ht="14.25" customHeight="1">
       <c r="G681" s="3"/>
     </row>
-    <row r="682" ht="14.25" customHeight="1">
+    <row r="682" spans="7:7" ht="14.25" customHeight="1">
       <c r="G682" s="3"/>
     </row>
-    <row r="683" ht="14.25" customHeight="1">
+    <row r="683" spans="7:7" ht="14.25" customHeight="1">
       <c r="G683" s="3"/>
     </row>
-    <row r="684" ht="14.25" customHeight="1">
+    <row r="684" spans="7:7" ht="14.25" customHeight="1">
       <c r="G684" s="3"/>
     </row>
-    <row r="685" ht="14.25" customHeight="1">
+    <row r="685" spans="7:7" ht="14.25" customHeight="1">
       <c r="G685" s="3"/>
     </row>
-    <row r="686" ht="14.25" customHeight="1">
+    <row r="686" spans="7:7" ht="14.25" customHeight="1">
       <c r="G686" s="3"/>
     </row>
-    <row r="687" ht="14.25" customHeight="1">
+    <row r="687" spans="7:7" ht="14.25" customHeight="1">
       <c r="G687" s="3"/>
     </row>
-    <row r="688" ht="14.25" customHeight="1">
+    <row r="688" spans="7:7" ht="14.25" customHeight="1">
       <c r="G688" s="3"/>
     </row>
-    <row r="689" ht="14.25" customHeight="1">
+    <row r="689" spans="7:7" ht="14.25" customHeight="1">
       <c r="G689" s="3"/>
     </row>
-    <row r="690" ht="14.25" customHeight="1">
+    <row r="690" spans="7:7" ht="14.25" customHeight="1">
       <c r="G690" s="3"/>
     </row>
-    <row r="691" ht="14.25" customHeight="1">
+    <row r="691" spans="7:7" ht="14.25" customHeight="1">
       <c r="G691" s="3"/>
     </row>
-    <row r="692" ht="14.25" customHeight="1">
+    <row r="692" spans="7:7" ht="14.25" customHeight="1">
       <c r="G692" s="3"/>
     </row>
-    <row r="693" ht="14.25" customHeight="1">
+    <row r="693" spans="7:7" ht="14.25" customHeight="1">
       <c r="G693" s="3"/>
     </row>
-    <row r="694" ht="14.25" customHeight="1">
+    <row r="694" spans="7:7" ht="14.25" customHeight="1">
       <c r="G694" s="3"/>
     </row>
-    <row r="695" ht="14.25" customHeight="1">
+    <row r="695" spans="7:7" ht="14.25" customHeight="1">
       <c r="G695" s="3"/>
     </row>
-    <row r="696" ht="14.25" customHeight="1">
+    <row r="696" spans="7:7" ht="14.25" customHeight="1">
       <c r="G696" s="3"/>
     </row>
-    <row r="697" ht="14.25" customHeight="1">
+    <row r="697" spans="7:7" ht="14.25" customHeight="1">
       <c r="G697" s="3"/>
     </row>
-    <row r="698" ht="14.25" customHeight="1">
+    <row r="698" spans="7:7" ht="14.25" customHeight="1">
       <c r="G698" s="3"/>
     </row>
-    <row r="699" ht="14.25" customHeight="1">
+    <row r="699" spans="7:7" ht="14.25" customHeight="1">
       <c r="G699" s="3"/>
     </row>
-    <row r="700" ht="14.25" customHeight="1">
+    <row r="700" spans="7:7" ht="14.25" customHeight="1">
       <c r="G700" s="3"/>
     </row>
-    <row r="701" ht="14.25" customHeight="1">
+    <row r="701" spans="7:7" ht="14.25" customHeight="1">
       <c r="G701" s="3"/>
     </row>
-    <row r="702" ht="14.25" customHeight="1">
+    <row r="702" spans="7:7" ht="14.25" customHeight="1">
       <c r="G702" s="3"/>
     </row>
-    <row r="703" ht="14.25" customHeight="1">
+    <row r="703" spans="7:7" ht="14.25" customHeight="1">
       <c r="G703" s="3"/>
     </row>
-    <row r="704" ht="14.25" customHeight="1">
+    <row r="704" spans="7:7" ht="14.25" customHeight="1">
       <c r="G704" s="3"/>
     </row>
-    <row r="705" ht="14.25" customHeight="1">
+    <row r="705" spans="7:7" ht="14.25" customHeight="1">
       <c r="G705" s="3"/>
     </row>
-    <row r="706" ht="14.25" customHeight="1">
+    <row r="706" spans="7:7" ht="14.25" customHeight="1">
       <c r="G706" s="3"/>
     </row>
-    <row r="707" ht="14.25" customHeight="1">
+    <row r="707" spans="7:7" ht="14.25" customHeight="1">
       <c r="G707" s="3"/>
     </row>
-    <row r="708" ht="14.25" customHeight="1">
+    <row r="708" spans="7:7" ht="14.25" customHeight="1">
       <c r="G708" s="3"/>
     </row>
-    <row r="709" ht="14.25" customHeight="1">
+    <row r="709" spans="7:7" ht="14.25" customHeight="1">
       <c r="G709" s="3"/>
     </row>
-    <row r="710" ht="14.25" customHeight="1">
+    <row r="710" spans="7:7" ht="14.25" customHeight="1">
       <c r="G710" s="3"/>
     </row>
-    <row r="711" ht="14.25" customHeight="1">
+    <row r="711" spans="7:7" ht="14.25" customHeight="1">
       <c r="G711" s="3"/>
     </row>
-    <row r="712" ht="14.25" customHeight="1">
+    <row r="712" spans="7:7" ht="14.25" customHeight="1">
       <c r="G712" s="3"/>
     </row>
-    <row r="713" ht="14.25" customHeight="1">
+    <row r="713" spans="7:7" ht="14.25" customHeight="1">
       <c r="G713" s="3"/>
     </row>
-    <row r="714" ht="14.25" customHeight="1">
+    <row r="714" spans="7:7" ht="14.25" customHeight="1">
       <c r="G714" s="3"/>
     </row>
-    <row r="715" ht="14.25" customHeight="1">
+    <row r="715" spans="7:7" ht="14.25" customHeight="1">
       <c r="G715" s="3"/>
     </row>
-    <row r="716" ht="14.25" customHeight="1">
+    <row r="716" spans="7:7" ht="14.25" customHeight="1">
       <c r="G716" s="3"/>
     </row>
-    <row r="717" ht="14.25" customHeight="1">
+    <row r="717" spans="7:7" ht="14.25" customHeight="1">
       <c r="G717" s="3"/>
     </row>
-    <row r="718" ht="14.25" customHeight="1">
+    <row r="718" spans="7:7" ht="14.25" customHeight="1">
       <c r="G718" s="3"/>
     </row>
-    <row r="719" ht="14.25" customHeight="1">
+    <row r="719" spans="7:7" ht="14.25" customHeight="1">
       <c r="G719" s="3"/>
     </row>
-    <row r="720" ht="14.25" customHeight="1">
+    <row r="720" spans="7:7" ht="14.25" customHeight="1">
       <c r="G720" s="3"/>
     </row>
-    <row r="721" ht="14.25" customHeight="1">
+    <row r="721" spans="7:7" ht="14.25" customHeight="1">
       <c r="G721" s="3"/>
     </row>
-    <row r="722" ht="14.25" customHeight="1">
+    <row r="722" spans="7:7" ht="14.25" customHeight="1">
       <c r="G722" s="3"/>
     </row>
-    <row r="723" ht="14.25" customHeight="1">
+    <row r="723" spans="7:7" ht="14.25" customHeight="1">
       <c r="G723" s="3"/>
     </row>
-    <row r="724" ht="14.25" customHeight="1">
+    <row r="724" spans="7:7" ht="14.25" customHeight="1">
       <c r="G724" s="3"/>
     </row>
-    <row r="725" ht="14.25" customHeight="1">
+    <row r="725" spans="7:7" ht="14.25" customHeight="1">
       <c r="G725" s="3"/>
     </row>
-    <row r="726" ht="14.25" customHeight="1">
+    <row r="726" spans="7:7" ht="14.25" customHeight="1">
       <c r="G726" s="3"/>
     </row>
-    <row r="727" ht="14.25" customHeight="1">
+    <row r="727" spans="7:7" ht="14.25" customHeight="1">
       <c r="G727" s="3"/>
     </row>
-    <row r="728" ht="14.25" customHeight="1">
+    <row r="728" spans="7:7" ht="14.25" customHeight="1">
       <c r="G728" s="3"/>
     </row>
-    <row r="729" ht="14.25" customHeight="1">
+    <row r="729" spans="7:7" ht="14.25" customHeight="1">
       <c r="G729" s="3"/>
     </row>
-    <row r="730" ht="14.25" customHeight="1">
+    <row r="730" spans="7:7" ht="14.25" customHeight="1">
       <c r="G730" s="3"/>
     </row>
-    <row r="731" ht="14.25" customHeight="1">
+    <row r="731" spans="7:7" ht="14.25" customHeight="1">
       <c r="G731" s="3"/>
     </row>
-    <row r="732" ht="14.25" customHeight="1">
+    <row r="732" spans="7:7" ht="14.25" customHeight="1">
       <c r="G732" s="3"/>
     </row>
-    <row r="733" ht="14.25" customHeight="1">
+    <row r="733" spans="7:7" ht="14.25" customHeight="1">
       <c r="G733" s="3"/>
     </row>
-    <row r="734" ht="14.25" customHeight="1">
+    <row r="734" spans="7:7" ht="14.25" customHeight="1">
       <c r="G734" s="3"/>
     </row>
-    <row r="735" ht="14.25" customHeight="1">
+    <row r="735" spans="7:7" ht="14.25" customHeight="1">
       <c r="G735" s="3"/>
     </row>
-    <row r="736" ht="14.25" customHeight="1">
+    <row r="736" spans="7:7" ht="14.25" customHeight="1">
       <c r="G736" s="3"/>
     </row>
-    <row r="737" ht="14.25" customHeight="1">
+    <row r="737" spans="7:7" ht="14.25" customHeight="1">
       <c r="G737" s="3"/>
     </row>
-    <row r="738" ht="14.25" customHeight="1">
+    <row r="738" spans="7:7" ht="14.25" customHeight="1">
       <c r="G738" s="3"/>
     </row>
-    <row r="739" ht="14.25" customHeight="1">
+    <row r="739" spans="7:7" ht="14.25" customHeight="1">
       <c r="G739" s="3"/>
     </row>
-    <row r="740" ht="14.25" customHeight="1">
+    <row r="740" spans="7:7" ht="14.25" customHeight="1">
       <c r="G740" s="3"/>
     </row>
-    <row r="741" ht="14.25" customHeight="1">
+    <row r="741" spans="7:7" ht="14.25" customHeight="1">
       <c r="G741" s="3"/>
     </row>
-    <row r="742" ht="14.25" customHeight="1">
+    <row r="742" spans="7:7" ht="14.25" customHeight="1">
       <c r="G742" s="3"/>
     </row>
-    <row r="743" ht="14.25" customHeight="1">
+    <row r="743" spans="7:7" ht="14.25" customHeight="1">
       <c r="G743" s="3"/>
     </row>
-    <row r="744" ht="14.25" customHeight="1">
+    <row r="744" spans="7:7" ht="14.25" customHeight="1">
       <c r="G744" s="3"/>
     </row>
-    <row r="745" ht="14.25" customHeight="1">
+    <row r="745" spans="7:7" ht="14.25" customHeight="1">
       <c r="G745" s="3"/>
     </row>
-    <row r="746" ht="14.25" customHeight="1">
+    <row r="746" spans="7:7" ht="14.25" customHeight="1">
       <c r="G746" s="3"/>
     </row>
-    <row r="747" ht="14.25" customHeight="1">
+    <row r="747" spans="7:7" ht="14.25" customHeight="1">
       <c r="G747" s="3"/>
     </row>
-    <row r="748" ht="14.25" customHeight="1">
+    <row r="748" spans="7:7" ht="14.25" customHeight="1">
       <c r="G748" s="3"/>
     </row>
-    <row r="749" ht="14.25" customHeight="1">
+    <row r="749" spans="7:7" ht="14.25" customHeight="1">
       <c r="G749" s="3"/>
     </row>
-    <row r="750" ht="14.25" customHeight="1">
+    <row r="750" spans="7:7" ht="14.25" customHeight="1">
       <c r="G750" s="3"/>
     </row>
-    <row r="751" ht="14.25" customHeight="1">
+    <row r="751" spans="7:7" ht="14.25" customHeight="1">
       <c r="G751" s="3"/>
     </row>
-    <row r="752" ht="14.25" customHeight="1">
+    <row r="752" spans="7:7" ht="14.25" customHeight="1">
       <c r="G752" s="3"/>
     </row>
-    <row r="753" ht="14.25" customHeight="1">
+    <row r="753" spans="7:7" ht="14.25" customHeight="1">
       <c r="G753" s="3"/>
     </row>
-    <row r="754" ht="14.25" customHeight="1">
+    <row r="754" spans="7:7" ht="14.25" customHeight="1">
       <c r="G754" s="3"/>
     </row>
-    <row r="755" ht="14.25" customHeight="1">
+    <row r="755" spans="7:7" ht="14.25" customHeight="1">
       <c r="G755" s="3"/>
     </row>
-    <row r="756" ht="14.25" customHeight="1">
+    <row r="756" spans="7:7" ht="14.25" customHeight="1">
       <c r="G756" s="3"/>
     </row>
-    <row r="757" ht="14.25" customHeight="1">
+    <row r="757" spans="7:7" ht="14.25" customHeight="1">
       <c r="G757" s="3"/>
     </row>
-    <row r="758" ht="14.25" customHeight="1">
+    <row r="758" spans="7:7" ht="14.25" customHeight="1">
       <c r="G758" s="3"/>
     </row>
-    <row r="759" ht="14.25" customHeight="1">
+    <row r="759" spans="7:7" ht="14.25" customHeight="1">
       <c r="G759" s="3"/>
     </row>
-    <row r="760" ht="14.25" customHeight="1">
+    <row r="760" spans="7:7" ht="14.25" customHeight="1">
       <c r="G760" s="3"/>
     </row>
-    <row r="761" ht="14.25" customHeight="1">
+    <row r="761" spans="7:7" ht="14.25" customHeight="1">
       <c r="G761" s="3"/>
     </row>
-    <row r="762" ht="14.25" customHeight="1">
+    <row r="762" spans="7:7" ht="14.25" customHeight="1">
       <c r="G762" s="3"/>
     </row>
-    <row r="763" ht="14.25" customHeight="1">
+    <row r="763" spans="7:7" ht="14.25" customHeight="1">
       <c r="G763" s="3"/>
     </row>
-    <row r="764" ht="14.25" customHeight="1">
+    <row r="764" spans="7:7" ht="14.25" customHeight="1">
       <c r="G764" s="3"/>
     </row>
-    <row r="765" ht="14.25" customHeight="1">
+    <row r="765" spans="7:7" ht="14.25" customHeight="1">
       <c r="G765" s="3"/>
     </row>
-    <row r="766" ht="14.25" customHeight="1">
+    <row r="766" spans="7:7" ht="14.25" customHeight="1">
       <c r="G766" s="3"/>
     </row>
-    <row r="767" ht="14.25" customHeight="1">
+    <row r="767" spans="7:7" ht="14.25" customHeight="1">
       <c r="G767" s="3"/>
     </row>
-    <row r="768" ht="14.25" customHeight="1">
+    <row r="768" spans="7:7" ht="14.25" customHeight="1">
       <c r="G768" s="3"/>
     </row>
-    <row r="769" ht="14.25" customHeight="1">
+    <row r="769" spans="7:7" ht="14.25" customHeight="1">
       <c r="G769" s="3"/>
     </row>
-    <row r="770" ht="14.25" customHeight="1">
+    <row r="770" spans="7:7" ht="14.25" customHeight="1">
       <c r="G770" s="3"/>
     </row>
-    <row r="771" ht="14.25" customHeight="1">
+    <row r="771" spans="7:7" ht="14.25" customHeight="1">
       <c r="G771" s="3"/>
     </row>
-    <row r="772" ht="14.25" customHeight="1">
+    <row r="772" spans="7:7" ht="14.25" customHeight="1">
       <c r="G772" s="3"/>
     </row>
-    <row r="773" ht="14.25" customHeight="1">
+    <row r="773" spans="7:7" ht="14.25" customHeight="1">
       <c r="G773" s="3"/>
     </row>
-    <row r="774" ht="14.25" customHeight="1">
+    <row r="774" spans="7:7" ht="14.25" customHeight="1">
       <c r="G774" s="3"/>
     </row>
-    <row r="775" ht="14.25" customHeight="1">
+    <row r="775" spans="7:7" ht="14.25" customHeight="1">
       <c r="G775" s="3"/>
     </row>
-    <row r="776" ht="14.25" customHeight="1">
+    <row r="776" spans="7:7" ht="14.25" customHeight="1">
       <c r="G776" s="3"/>
     </row>
-    <row r="777" ht="14.25" customHeight="1">
+    <row r="777" spans="7:7" ht="14.25" customHeight="1">
       <c r="G777" s="3"/>
     </row>
-    <row r="778" ht="14.25" customHeight="1">
+    <row r="778" spans="7:7" ht="14.25" customHeight="1">
       <c r="G778" s="3"/>
     </row>
-    <row r="779" ht="14.25" customHeight="1">
+    <row r="779" spans="7:7" ht="14.25" customHeight="1">
       <c r="G779" s="3"/>
     </row>
-    <row r="780" ht="14.25" customHeight="1">
+    <row r="780" spans="7:7" ht="14.25" customHeight="1">
       <c r="G780" s="3"/>
     </row>
-    <row r="781" ht="14.25" customHeight="1">
+    <row r="781" spans="7:7" ht="14.25" customHeight="1">
       <c r="G781" s="3"/>
     </row>
-    <row r="782" ht="14.25" customHeight="1">
+    <row r="782" spans="7:7" ht="14.25" customHeight="1">
       <c r="G782" s="3"/>
     </row>
-    <row r="783" ht="14.25" customHeight="1">
+    <row r="783" spans="7:7" ht="14.25" customHeight="1">
       <c r="G783" s="3"/>
     </row>
-    <row r="784" ht="14.25" customHeight="1">
+    <row r="784" spans="7:7" ht="14.25" customHeight="1">
       <c r="G784" s="3"/>
     </row>
-    <row r="785" ht="14.25" customHeight="1">
+    <row r="785" spans="7:7" ht="14.25" customHeight="1">
       <c r="G785" s="3"/>
     </row>
-    <row r="786" ht="14.25" customHeight="1">
+    <row r="786" spans="7:7" ht="14.25" customHeight="1">
       <c r="G786" s="3"/>
     </row>
-    <row r="787" ht="14.25" customHeight="1">
+    <row r="787" spans="7:7" ht="14.25" customHeight="1">
       <c r="G787" s="3"/>
     </row>
-    <row r="788" ht="14.25" customHeight="1">
+    <row r="788" spans="7:7" ht="14.25" customHeight="1">
       <c r="G788" s="3"/>
     </row>
-    <row r="789" ht="14.25" customHeight="1">
+    <row r="789" spans="7:7" ht="14.25" customHeight="1">
       <c r="G789" s="3"/>
     </row>
-    <row r="790" ht="14.25" customHeight="1">
+    <row r="790" spans="7:7" ht="14.25" customHeight="1">
       <c r="G790" s="3"/>
     </row>
-    <row r="791" ht="14.25" customHeight="1">
+    <row r="791" spans="7:7" ht="14.25" customHeight="1">
       <c r="G791" s="3"/>
     </row>
-    <row r="792" ht="14.25" customHeight="1">
+    <row r="792" spans="7:7" ht="14.25" customHeight="1">
       <c r="G792" s="3"/>
     </row>
-    <row r="793" ht="14.25" customHeight="1">
+    <row r="793" spans="7:7" ht="14.25" customHeight="1">
       <c r="G793" s="3"/>
     </row>
-    <row r="794" ht="14.25" customHeight="1">
+    <row r="794" spans="7:7" ht="14.25" customHeight="1">
       <c r="G794" s="3"/>
     </row>
-    <row r="795" ht="14.25" customHeight="1">
+    <row r="795" spans="7:7" ht="14.25" customHeight="1">
       <c r="G795" s="3"/>
     </row>
-    <row r="796" ht="14.25" customHeight="1">
+    <row r="796" spans="7:7" ht="14.25" customHeight="1">
       <c r="G796" s="3"/>
     </row>
-    <row r="797" ht="14.25" customHeight="1">
+    <row r="797" spans="7:7" ht="14.25" customHeight="1">
       <c r="G797" s="3"/>
     </row>
-    <row r="798" ht="14.25" customHeight="1">
+    <row r="798" spans="7:7" ht="14.25" customHeight="1">
       <c r="G798" s="3"/>
     </row>
-    <row r="799" ht="14.25" customHeight="1">
+    <row r="799" spans="7:7" ht="14.25" customHeight="1">
       <c r="G799" s="3"/>
     </row>
-    <row r="800" ht="14.25" customHeight="1">
+    <row r="800" spans="7:7" ht="14.25" customHeight="1">
       <c r="G800" s="3"/>
     </row>
-    <row r="801" ht="14.25" customHeight="1">
+    <row r="801" spans="7:7" ht="14.25" customHeight="1">
       <c r="G801" s="3"/>
     </row>
-    <row r="802" ht="14.25" customHeight="1">
+    <row r="802" spans="7:7" ht="14.25" customHeight="1">
       <c r="G802" s="3"/>
     </row>
-    <row r="803" ht="14.25" customHeight="1">
+    <row r="803" spans="7:7" ht="14.25" customHeight="1">
       <c r="G803" s="3"/>
     </row>
-    <row r="804" ht="14.25" customHeight="1">
+    <row r="804" spans="7:7" ht="14.25" customHeight="1">
       <c r="G804" s="3"/>
     </row>
-    <row r="805" ht="14.25" customHeight="1">
+    <row r="805" spans="7:7" ht="14.25" customHeight="1">
       <c r="G805" s="3"/>
     </row>
-    <row r="806" ht="14.25" customHeight="1">
+    <row r="806" spans="7:7" ht="14.25" customHeight="1">
       <c r="G806" s="3"/>
     </row>
-    <row r="807" ht="14.25" customHeight="1">
+    <row r="807" spans="7:7" ht="14.25" customHeight="1">
       <c r="G807" s="3"/>
     </row>
-    <row r="808" ht="14.25" customHeight="1">
+    <row r="808" spans="7:7" ht="14.25" customHeight="1">
       <c r="G808" s="3"/>
     </row>
-    <row r="809" ht="14.25" customHeight="1">
+    <row r="809" spans="7:7" ht="14.25" customHeight="1">
       <c r="G809" s="3"/>
     </row>
-    <row r="810" ht="14.25" customHeight="1">
+    <row r="810" spans="7:7" ht="14.25" customHeight="1">
       <c r="G810" s="3"/>
     </row>
-    <row r="811" ht="14.25" customHeight="1">
+    <row r="811" spans="7:7" ht="14.25" customHeight="1">
       <c r="G811" s="3"/>
     </row>
-    <row r="812" ht="14.25" customHeight="1">
+    <row r="812" spans="7:7" ht="14.25" customHeight="1">
       <c r="G812" s="3"/>
     </row>
-    <row r="813" ht="14.25" customHeight="1">
+    <row r="813" spans="7:7" ht="14.25" customHeight="1">
       <c r="G813" s="3"/>
     </row>
-    <row r="814" ht="14.25" customHeight="1">
+    <row r="814" spans="7:7" ht="14.25" customHeight="1">
       <c r="G814" s="3"/>
     </row>
-    <row r="815" ht="14.25" customHeight="1">
+    <row r="815" spans="7:7" ht="14.25" customHeight="1">
       <c r="G815" s="3"/>
     </row>
-    <row r="816" ht="14.25" customHeight="1">
+    <row r="816" spans="7:7" ht="14.25" customHeight="1">
       <c r="G816" s="3"/>
     </row>
-    <row r="817" ht="14.25" customHeight="1">
+    <row r="817" spans="7:7" ht="14.25" customHeight="1">
       <c r="G817" s="3"/>
     </row>
-    <row r="818" ht="14.25" customHeight="1">
+    <row r="818" spans="7:7" ht="14.25" customHeight="1">
       <c r="G818" s="3"/>
     </row>
-    <row r="819" ht="14.25" customHeight="1">
+    <row r="819" spans="7:7" ht="14.25" customHeight="1">
       <c r="G819" s="3"/>
     </row>
-    <row r="820" ht="14.25" customHeight="1">
+    <row r="820" spans="7:7" ht="14.25" customHeight="1">
       <c r="G820" s="3"/>
     </row>
-    <row r="821" ht="14.25" customHeight="1">
+    <row r="821" spans="7:7" ht="14.25" customHeight="1">
       <c r="G821" s="3"/>
     </row>
-    <row r="822" ht="14.25" customHeight="1">
+    <row r="822" spans="7:7" ht="14.25" customHeight="1">
       <c r="G822" s="3"/>
     </row>
-    <row r="823" ht="14.25" customHeight="1">
+    <row r="823" spans="7:7" ht="14.25" customHeight="1">
       <c r="G823" s="3"/>
     </row>
-    <row r="824" ht="14.25" customHeight="1">
+    <row r="824" spans="7:7" ht="14.25" customHeight="1">
       <c r="G824" s="3"/>
     </row>
-    <row r="825" ht="14.25" customHeight="1">
+    <row r="825" spans="7:7" ht="14.25" customHeight="1">
       <c r="G825" s="3"/>
     </row>
-    <row r="826" ht="14.25" customHeight="1">
+    <row r="826" spans="7:7" ht="14.25" customHeight="1">
       <c r="G826" s="3"/>
     </row>
-    <row r="827" ht="14.25" customHeight="1">
+    <row r="827" spans="7:7" ht="14.25" customHeight="1">
       <c r="G827" s="3"/>
     </row>
-    <row r="828" ht="14.25" customHeight="1">
+    <row r="828" spans="7:7" ht="14.25" customHeight="1">
       <c r="G828" s="3"/>
     </row>
-    <row r="829" ht="14.25" customHeight="1">
+    <row r="829" spans="7:7" ht="14.25" customHeight="1">
       <c r="G829" s="3"/>
     </row>
-    <row r="830" ht="14.25" customHeight="1">
+    <row r="830" spans="7:7" ht="14.25" customHeight="1">
       <c r="G830" s="3"/>
     </row>
-    <row r="831" ht="14.25" customHeight="1">
+    <row r="831" spans="7:7" ht="14.25" customHeight="1">
       <c r="G831" s="3"/>
     </row>
-    <row r="832" ht="14.25" customHeight="1">
+    <row r="832" spans="7:7" ht="14.25" customHeight="1">
       <c r="G832" s="3"/>
     </row>
-    <row r="833" ht="14.25" customHeight="1">
+    <row r="833" spans="7:7" ht="14.25" customHeight="1">
       <c r="G833" s="3"/>
     </row>
-    <row r="834" ht="14.25" customHeight="1">
+    <row r="834" spans="7:7" ht="14.25" customHeight="1">
       <c r="G834" s="3"/>
     </row>
-    <row r="835" ht="14.25" customHeight="1">
+    <row r="835" spans="7:7" ht="14.25" customHeight="1">
       <c r="G835" s="3"/>
     </row>
-    <row r="836" ht="14.25" customHeight="1">
+    <row r="836" spans="7:7" ht="14.25" customHeight="1">
       <c r="G836" s="3"/>
     </row>
-    <row r="837" ht="14.25" customHeight="1">
+    <row r="837" spans="7:7" ht="14.25" customHeight="1">
       <c r="G837" s="3"/>
     </row>
-    <row r="838" ht="14.25" customHeight="1">
+    <row r="838" spans="7:7" ht="14.25" customHeight="1">
       <c r="G838" s="3"/>
     </row>
-    <row r="839" ht="14.25" customHeight="1">
+    <row r="839" spans="7:7" ht="14.25" customHeight="1">
       <c r="G839" s="3"/>
     </row>
-    <row r="840" ht="14.25" customHeight="1">
+    <row r="840" spans="7:7" ht="14.25" customHeight="1">
       <c r="G840" s="3"/>
     </row>
-    <row r="841" ht="14.25" customHeight="1">
+    <row r="841" spans="7:7" ht="14.25" customHeight="1">
       <c r="G841" s="3"/>
     </row>
-    <row r="842" ht="14.25" customHeight="1">
+    <row r="842" spans="7:7" ht="14.25" customHeight="1">
       <c r="G842" s="3"/>
     </row>
-    <row r="843" ht="14.25" customHeight="1">
+    <row r="843" spans="7:7" ht="14.25" customHeight="1">
       <c r="G843" s="3"/>
     </row>
-    <row r="844" ht="14.25" customHeight="1">
+    <row r="844" spans="7:7" ht="14.25" customHeight="1">
       <c r="G844" s="3"/>
     </row>
-    <row r="845" ht="14.25" customHeight="1">
+    <row r="845" spans="7:7" ht="14.25" customHeight="1">
       <c r="G845" s="3"/>
     </row>
-    <row r="846" ht="14.25" customHeight="1">
+    <row r="846" spans="7:7" ht="14.25" customHeight="1">
       <c r="G846" s="3"/>
     </row>
-    <row r="847" ht="14.25" customHeight="1">
+    <row r="847" spans="7:7" ht="14.25" customHeight="1">
       <c r="G847" s="3"/>
     </row>
-    <row r="848" ht="14.25" customHeight="1">
+    <row r="848" spans="7:7" ht="14.25" customHeight="1">
       <c r="G848" s="3"/>
     </row>
-    <row r="849" ht="14.25" customHeight="1">
+    <row r="849" spans="7:7" ht="14.25" customHeight="1">
       <c r="G849" s="3"/>
     </row>
-    <row r="850" ht="14.25" customHeight="1">
+    <row r="850" spans="7:7" ht="14.25" customHeight="1">
       <c r="G850" s="3"/>
     </row>
-    <row r="851" ht="14.25" customHeight="1">
+    <row r="851" spans="7:7" ht="14.25" customHeight="1">
       <c r="G851" s="3"/>
     </row>
-    <row r="852" ht="14.25" customHeight="1">
+    <row r="852" spans="7:7" ht="14.25" customHeight="1">
       <c r="G852" s="3"/>
     </row>
-    <row r="853" ht="14.25" customHeight="1">
+    <row r="853" spans="7:7" ht="14.25" customHeight="1">
       <c r="G853" s="3"/>
     </row>
-    <row r="854" ht="14.25" customHeight="1">
+    <row r="854" spans="7:7" ht="14.25" customHeight="1">
       <c r="G854" s="3"/>
     </row>
-    <row r="855" ht="14.25" customHeight="1">
+    <row r="855" spans="7:7" ht="14.25" customHeight="1">
       <c r="G855" s="3"/>
     </row>
-    <row r="856" ht="14.25" customHeight="1">
+    <row r="856" spans="7:7" ht="14.25" customHeight="1">
       <c r="G856" s="3"/>
     </row>
-    <row r="857" ht="14.25" customHeight="1">
+    <row r="857" spans="7:7" ht="14.25" customHeight="1">
       <c r="G857" s="3"/>
     </row>
-    <row r="858" ht="14.25" customHeight="1">
+    <row r="858" spans="7:7" ht="14.25" customHeight="1">
       <c r="G858" s="3"/>
     </row>
-    <row r="859" ht="14.25" customHeight="1">
+    <row r="859" spans="7:7" ht="14.25" customHeight="1">
       <c r="G859" s="3"/>
     </row>
-    <row r="860" ht="14.25" customHeight="1">
+    <row r="860" spans="7:7" ht="14.25" customHeight="1">
       <c r="G860" s="3"/>
     </row>
-    <row r="861" ht="14.25" customHeight="1">
+    <row r="861" spans="7:7" ht="14.25" customHeight="1">
       <c r="G861" s="3"/>
     </row>
-    <row r="862" ht="14.25" customHeight="1">
+    <row r="862" spans="7:7" ht="14.25" customHeight="1">
       <c r="G862" s="3"/>
     </row>
-    <row r="863" ht="14.25" customHeight="1">
+    <row r="863" spans="7:7" ht="14.25" customHeight="1">
       <c r="G863" s="3"/>
     </row>
-    <row r="864" ht="14.25" customHeight="1">
+    <row r="864" spans="7:7" ht="14.25" customHeight="1">
       <c r="G864" s="3"/>
     </row>
-    <row r="865" ht="14.25" customHeight="1">
+    <row r="865" spans="7:7" ht="14.25" customHeight="1">
       <c r="G865" s="3"/>
     </row>
-    <row r="866" ht="14.25" customHeight="1">
+    <row r="866" spans="7:7" ht="14.25" customHeight="1">
       <c r="G866" s="3"/>
     </row>
-    <row r="867" ht="14.25" customHeight="1">
+    <row r="867" spans="7:7" ht="14.25" customHeight="1">
       <c r="G867" s="3"/>
     </row>
-    <row r="868" ht="14.25" customHeight="1">
+    <row r="868" spans="7:7" ht="14.25" customHeight="1">
       <c r="G868" s="3"/>
     </row>
-    <row r="869" ht="14.25" customHeight="1">
+    <row r="869" spans="7:7" ht="14.25" customHeight="1">
       <c r="G869" s="3"/>
     </row>
-    <row r="870" ht="14.25" customHeight="1">
+    <row r="870" spans="7:7" ht="14.25" customHeight="1">
       <c r="G870" s="3"/>
     </row>
-    <row r="871" ht="14.25" customHeight="1">
+    <row r="871" spans="7:7" ht="14.25" customHeight="1">
       <c r="G871" s="3"/>
     </row>
-    <row r="872" ht="14.25" customHeight="1">
+    <row r="872" spans="7:7" ht="14.25" customHeight="1">
       <c r="G872" s="3"/>
     </row>
-    <row r="873" ht="14.25" customHeight="1">
+    <row r="873" spans="7:7" ht="14.25" customHeight="1">
       <c r="G873" s="3"/>
     </row>
-    <row r="874" ht="14.25" customHeight="1">
+    <row r="874" spans="7:7" ht="14.25" customHeight="1">
       <c r="G874" s="3"/>
     </row>
-    <row r="875" ht="14.25" customHeight="1">
+    <row r="875" spans="7:7" ht="14.25" customHeight="1">
       <c r="G875" s="3"/>
     </row>
-    <row r="876" ht="14.25" customHeight="1">
+    <row r="876" spans="7:7" ht="14.25" customHeight="1">
       <c r="G876" s="3"/>
     </row>
-    <row r="877" ht="14.25" customHeight="1">
+    <row r="877" spans="7:7" ht="14.25" customHeight="1">
       <c r="G877" s="3"/>
     </row>
-    <row r="878" ht="14.25" customHeight="1">
+    <row r="878" spans="7:7" ht="14.25" customHeight="1">
       <c r="G878" s="3"/>
     </row>
-    <row r="879" ht="14.25" customHeight="1">
+    <row r="879" spans="7:7" ht="14.25" customHeight="1">
       <c r="G879" s="3"/>
     </row>
-    <row r="880" ht="14.25" customHeight="1">
+    <row r="880" spans="7:7" ht="14.25" customHeight="1">
       <c r="G880" s="3"/>
     </row>
-    <row r="881" ht="14.25" customHeight="1">
+    <row r="881" spans="7:7" ht="14.25" customHeight="1">
       <c r="G881" s="3"/>
     </row>
-    <row r="882" ht="14.25" customHeight="1">
+    <row r="882" spans="7:7" ht="14.25" customHeight="1">
       <c r="G882" s="3"/>
     </row>
-    <row r="883" ht="14.25" customHeight="1">
+    <row r="883" spans="7:7" ht="14.25" customHeight="1">
       <c r="G883" s="3"/>
     </row>
-    <row r="884" ht="14.25" customHeight="1">
+    <row r="884" spans="7:7" ht="14.25" customHeight="1">
       <c r="G884" s="3"/>
     </row>
-    <row r="885" ht="14.25" customHeight="1">
+    <row r="885" spans="7:7" ht="14.25" customHeight="1">
       <c r="G885" s="3"/>
     </row>
-    <row r="886" ht="14.25" customHeight="1">
+    <row r="886" spans="7:7" ht="14.25" customHeight="1">
       <c r="G886" s="3"/>
     </row>
-    <row r="887" ht="14.25" customHeight="1">
+    <row r="887" spans="7:7" ht="14.25" customHeight="1">
       <c r="G887" s="3"/>
     </row>
-    <row r="888" ht="14.25" customHeight="1">
+    <row r="888" spans="7:7" ht="14.25" customHeight="1">
       <c r="G888" s="3"/>
     </row>
-    <row r="889" ht="14.25" customHeight="1">
+    <row r="889" spans="7:7" ht="14.25" customHeight="1">
       <c r="G889" s="3"/>
     </row>
-    <row r="890" ht="14.25" customHeight="1">
+    <row r="890" spans="7:7" ht="14.25" customHeight="1">
       <c r="G890" s="3"/>
     </row>
-    <row r="891" ht="14.25" customHeight="1">
+    <row r="891" spans="7:7" ht="14.25" customHeight="1">
       <c r="G891" s="3"/>
     </row>
-    <row r="892" ht="14.25" customHeight="1">
+    <row r="892" spans="7:7" ht="14.25" customHeight="1">
       <c r="G892" s="3"/>
     </row>
-    <row r="893" ht="14.25" customHeight="1">
+    <row r="893" spans="7:7" ht="14.25" customHeight="1">
       <c r="G893" s="3"/>
     </row>
-    <row r="894" ht="14.25" customHeight="1">
+    <row r="894" spans="7:7" ht="14.25" customHeight="1">
       <c r="G894" s="3"/>
     </row>
-    <row r="895" ht="14.25" customHeight="1">
+    <row r="895" spans="7:7" ht="14.25" customHeight="1">
       <c r="G895" s="3"/>
     </row>
-    <row r="896" ht="14.25" customHeight="1">
+    <row r="896" spans="7:7" ht="14.25" customHeight="1">
       <c r="G896" s="3"/>
     </row>
-    <row r="897" ht="14.25" customHeight="1">
+    <row r="897" spans="7:7" ht="14.25" customHeight="1">
       <c r="G897" s="3"/>
     </row>
-    <row r="898" ht="14.25" customHeight="1">
+    <row r="898" spans="7:7" ht="14.25" customHeight="1">
       <c r="G898" s="3"/>
     </row>
-    <row r="899" ht="14.25" customHeight="1">
+    <row r="899" spans="7:7" ht="14.25" customHeight="1">
       <c r="G899" s="3"/>
     </row>
-    <row r="900" ht="14.25" customHeight="1">
+    <row r="900" spans="7:7" ht="14.25" customHeight="1">
       <c r="G900" s="3"/>
     </row>
-    <row r="901" ht="14.25" customHeight="1">
+    <row r="901" spans="7:7" ht="14.25" customHeight="1">
       <c r="G901" s="3"/>
     </row>
-    <row r="902" ht="14.25" customHeight="1">
+    <row r="902" spans="7:7" ht="14.25" customHeight="1">
       <c r="G902" s="3"/>
     </row>
-    <row r="903" ht="14.25" customHeight="1">
+    <row r="903" spans="7:7" ht="14.25" customHeight="1">
       <c r="G903" s="3"/>
     </row>
-    <row r="904" ht="14.25" customHeight="1">
+    <row r="904" spans="7:7" ht="14.25" customHeight="1">
       <c r="G904" s="3"/>
     </row>
-    <row r="905" ht="14.25" customHeight="1">
+    <row r="905" spans="7:7" ht="14.25" customHeight="1">
       <c r="G905" s="3"/>
     </row>
-    <row r="906" ht="14.25" customHeight="1">
+    <row r="906" spans="7:7" ht="14.25" customHeight="1">
       <c r="G906" s="3"/>
     </row>
-    <row r="907" ht="14.25" customHeight="1">
+    <row r="907" spans="7:7" ht="14.25" customHeight="1">
       <c r="G907" s="3"/>
     </row>
-    <row r="908" ht="14.25" customHeight="1">
+    <row r="908" spans="7:7" ht="14.25" customHeight="1">
       <c r="G908" s="3"/>
     </row>
-    <row r="909" ht="14.25" customHeight="1">
+    <row r="909" spans="7:7" ht="14.25" customHeight="1">
       <c r="G909" s="3"/>
     </row>
-    <row r="910" ht="14.25" customHeight="1">
+    <row r="910" spans="7:7" ht="14.25" customHeight="1">
       <c r="G910" s="3"/>
     </row>
-    <row r="911" ht="14.25" customHeight="1">
+    <row r="911" spans="7:7" ht="14.25" customHeight="1">
       <c r="G911" s="3"/>
     </row>
-    <row r="912" ht="14.25" customHeight="1">
+    <row r="912" spans="7:7" ht="14.25" customHeight="1">
       <c r="G912" s="3"/>
     </row>
-    <row r="913" ht="14.25" customHeight="1">
+    <row r="913" spans="7:7" ht="14.25" customHeight="1">
       <c r="G913" s="3"/>
     </row>
-    <row r="914" ht="14.25" customHeight="1">
+    <row r="914" spans="7:7" ht="14.25" customHeight="1">
       <c r="G914" s="3"/>
     </row>
-    <row r="915" ht="14.25" customHeight="1">
+    <row r="915" spans="7:7" ht="14.25" customHeight="1">
       <c r="G915" s="3"/>
     </row>
-    <row r="916" ht="14.25" customHeight="1">
+    <row r="916" spans="7:7" ht="14.25" customHeight="1">
       <c r="G916" s="3"/>
     </row>
-    <row r="917" ht="14.25" customHeight="1">
+    <row r="917" spans="7:7" ht="14.25" customHeight="1">
       <c r="G917" s="3"/>
     </row>
-    <row r="918" ht="14.25" customHeight="1">
+    <row r="918" spans="7:7" ht="14.25" customHeight="1">
       <c r="G918" s="3"/>
     </row>
-    <row r="919" ht="14.25" customHeight="1">
+    <row r="919" spans="7:7" ht="14.25" customHeight="1">
       <c r="G919" s="3"/>
     </row>
-    <row r="920" ht="14.25" customHeight="1">
+    <row r="920" spans="7:7" ht="14.25" customHeight="1">
       <c r="G920" s="3"/>
     </row>
-    <row r="921" ht="14.25" customHeight="1">
+    <row r="921" spans="7:7" ht="14.25" customHeight="1">
       <c r="G921" s="3"/>
     </row>
-    <row r="922" ht="14.25" customHeight="1">
+    <row r="922" spans="7:7" ht="14.25" customHeight="1">
       <c r="G922" s="3"/>
     </row>
-    <row r="923" ht="14.25" customHeight="1">
+    <row r="923" spans="7:7" ht="14.25" customHeight="1">
       <c r="G923" s="3"/>
     </row>
-    <row r="924" ht="14.25" customHeight="1">
+    <row r="924" spans="7:7" ht="14.25" customHeight="1">
       <c r="G924" s="3"/>
     </row>
-    <row r="925" ht="14.25" customHeight="1">
+    <row r="925" spans="7:7" ht="14.25" customHeight="1">
       <c r="G925" s="3"/>
     </row>
-    <row r="926" ht="14.25" customHeight="1">
+    <row r="926" spans="7:7" ht="14.25" customHeight="1">
       <c r="G926" s="3"/>
     </row>
-    <row r="927" ht="14.25" customHeight="1">
+    <row r="927" spans="7:7" ht="14.25" customHeight="1">
       <c r="G927" s="3"/>
     </row>
-    <row r="928" ht="14.25" customHeight="1">
+    <row r="928" spans="7:7" ht="14.25" customHeight="1">
       <c r="G928" s="3"/>
     </row>
-    <row r="929" ht="14.25" customHeight="1">
+    <row r="929" spans="7:7" ht="14.25" customHeight="1">
       <c r="G929" s="3"/>
     </row>
-    <row r="930" ht="14.25" customHeight="1">
+    <row r="930" spans="7:7" ht="14.25" customHeight="1">
       <c r="G930" s="3"/>
     </row>
-    <row r="931" ht="14.25" customHeight="1">
+    <row r="931" spans="7:7" ht="14.25" customHeight="1">
       <c r="G931" s="3"/>
     </row>
-    <row r="932" ht="14.25" customHeight="1">
+    <row r="932" spans="7:7" ht="14.25" customHeight="1">
       <c r="G932" s="3"/>
     </row>
-    <row r="933" ht="14.25" customHeight="1">
+    <row r="933" spans="7:7" ht="14.25" customHeight="1">
       <c r="G933" s="3"/>
     </row>
-    <row r="934" ht="14.25" customHeight="1">
+    <row r="934" spans="7:7" ht="14.25" customHeight="1">
       <c r="G934" s="3"/>
     </row>
-    <row r="935" ht="14.25" customHeight="1">
+    <row r="935" spans="7:7" ht="14.25" customHeight="1">
       <c r="G935" s="3"/>
     </row>
-    <row r="936" ht="14.25" customHeight="1">
+    <row r="936" spans="7:7" ht="14.25" customHeight="1">
       <c r="G936" s="3"/>
     </row>
-    <row r="937" ht="14.25" customHeight="1">
+    <row r="937" spans="7:7" ht="14.25" customHeight="1">
       <c r="G937" s="3"/>
     </row>
-    <row r="938" ht="14.25" customHeight="1">
+    <row r="938" spans="7:7" ht="14.25" customHeight="1">
       <c r="G938" s="3"/>
     </row>
-    <row r="939" ht="14.25" customHeight="1">
+    <row r="939" spans="7:7" ht="14.25" customHeight="1">
       <c r="G939" s="3"/>
     </row>
-    <row r="940" ht="14.25" customHeight="1">
+    <row r="940" spans="7:7" ht="14.25" customHeight="1">
       <c r="G940" s="3"/>
     </row>
-    <row r="941" ht="14.25" customHeight="1">
+    <row r="941" spans="7:7" ht="14.25" customHeight="1">
       <c r="G941" s="3"/>
     </row>
-    <row r="942" ht="14.25" customHeight="1">
+    <row r="942" spans="7:7" ht="14.25" customHeight="1">
       <c r="G942" s="3"/>
     </row>
-    <row r="943" ht="14.25" customHeight="1">
+    <row r="943" spans="7:7" ht="14.25" customHeight="1">
       <c r="G943" s="3"/>
     </row>
-    <row r="944" ht="14.25" customHeight="1">
+    <row r="944" spans="7:7" ht="14.25" customHeight="1">
       <c r="G944" s="3"/>
     </row>
-    <row r="945" ht="14.25" customHeight="1">
+    <row r="945" spans="7:7" ht="14.25" customHeight="1">
       <c r="G945" s="3"/>
     </row>
-    <row r="946" ht="14.25" customHeight="1">
+    <row r="946" spans="7:7" ht="14.25" customHeight="1">
       <c r="G946" s="3"/>
     </row>
-    <row r="947" ht="14.25" customHeight="1">
+    <row r="947" spans="7:7" ht="14.25" customHeight="1">
       <c r="G947" s="3"/>
     </row>
-    <row r="948" ht="14.25" customHeight="1">
+    <row r="948" spans="7:7" ht="14.25" customHeight="1">
       <c r="G948" s="3"/>
     </row>
-    <row r="949" ht="14.25" customHeight="1">
+    <row r="949" spans="7:7" ht="14.25" customHeight="1">
       <c r="G949" s="3"/>
     </row>
-    <row r="950" ht="14.25" customHeight="1">
+    <row r="950" spans="7:7" ht="14.25" customHeight="1">
       <c r="G950" s="3"/>
     </row>
-    <row r="951" ht="14.25" customHeight="1">
+    <row r="951" spans="7:7" ht="14.25" customHeight="1">
       <c r="G951" s="3"/>
     </row>
-    <row r="952" ht="14.25" customHeight="1">
+    <row r="952" spans="7:7" ht="14.25" customHeight="1">
       <c r="G952" s="3"/>
     </row>
-    <row r="953" ht="14.25" customHeight="1">
+    <row r="953" spans="7:7" ht="14.25" customHeight="1">
       <c r="G953" s="3"/>
     </row>
-    <row r="954" ht="14.25" customHeight="1">
+    <row r="954" spans="7:7" ht="14.25" customHeight="1">
       <c r="G954" s="3"/>
     </row>
-    <row r="955" ht="14.25" customHeight="1">
+    <row r="955" spans="7:7" ht="14.25" customHeight="1">
       <c r="G955" s="3"/>
     </row>
-    <row r="956" ht="14.25" customHeight="1">
+    <row r="956" spans="7:7" ht="14.25" customHeight="1">
       <c r="G956" s="3"/>
     </row>
-    <row r="957" ht="14.25" customHeight="1">
+    <row r="957" spans="7:7" ht="14.25" customHeight="1">
       <c r="G957" s="3"/>
     </row>
-    <row r="958" ht="14.25" customHeight="1">
+    <row r="958" spans="7:7" ht="14.25" customHeight="1">
       <c r="G958" s="3"/>
     </row>
-    <row r="959" ht="14.25" customHeight="1">
+    <row r="959" spans="7:7" ht="14.25" customHeight="1">
       <c r="G959" s="3"/>
     </row>
-    <row r="960" ht="14.25" customHeight="1">
+    <row r="960" spans="7:7" ht="14.25" customHeight="1">
       <c r="G960" s="3"/>
     </row>
-    <row r="961" ht="14.25" customHeight="1">
+    <row r="961" spans="7:7" ht="14.25" customHeight="1">
       <c r="G961" s="3"/>
     </row>
-    <row r="962" ht="14.25" customHeight="1">
+    <row r="962" spans="7:7" ht="14.25" customHeight="1">
       <c r="G962" s="3"/>
     </row>
-    <row r="963" ht="14.25" customHeight="1">
+    <row r="963" spans="7:7" ht="14.25" customHeight="1">
       <c r="G963" s="3"/>
     </row>
-    <row r="964" ht="14.25" customHeight="1">
+    <row r="964" spans="7:7" ht="14.25" customHeight="1">
       <c r="G964" s="3"/>
     </row>
-    <row r="965" ht="14.25" customHeight="1">
+    <row r="965" spans="7:7" ht="14.25" customHeight="1">
       <c r="G965" s="3"/>
     </row>
-    <row r="966" ht="14.25" customHeight="1">
+    <row r="966" spans="7:7" ht="14.25" customHeight="1">
       <c r="G966" s="3"/>
     </row>
-    <row r="967" ht="14.25" customHeight="1">
+    <row r="967" spans="7:7" ht="14.25" customHeight="1">
       <c r="G967" s="3"/>
     </row>
-    <row r="968" ht="14.25" customHeight="1">
+    <row r="968" spans="7:7" ht="14.25" customHeight="1">
       <c r="G968" s="3"/>
     </row>
-    <row r="969" ht="14.25" customHeight="1">
+    <row r="969" spans="7:7" ht="14.25" customHeight="1">
       <c r="G969" s="3"/>
     </row>
-    <row r="970" ht="14.25" customHeight="1">
+    <row r="970" spans="7:7" ht="14.25" customHeight="1">
       <c r="G970" s="3"/>
     </row>
-    <row r="971" ht="14.25" customHeight="1">
+    <row r="971" spans="7:7" ht="14.25" customHeight="1">
       <c r="G971" s="3"/>
     </row>
-    <row r="972" ht="14.25" customHeight="1">
+    <row r="972" spans="7:7" ht="14.25" customHeight="1">
       <c r="G972" s="3"/>
     </row>
-    <row r="973" ht="14.25" customHeight="1">
+    <row r="973" spans="7:7" ht="14.25" customHeight="1">
       <c r="G973" s="3"/>
     </row>
-    <row r="974" ht="14.25" customHeight="1">
+    <row r="974" spans="7:7" ht="14.25" customHeight="1">
       <c r="G974" s="3"/>
     </row>
-    <row r="975" ht="14.25" customHeight="1">
+    <row r="975" spans="7:7" ht="14.25" customHeight="1">
       <c r="G975" s="3"/>
     </row>
-    <row r="976" ht="14.25" customHeight="1">
+    <row r="976" spans="7:7" ht="14.25" customHeight="1">
       <c r="G976" s="3"/>
     </row>
-    <row r="977" ht="14.25" customHeight="1">
+    <row r="977" spans="7:7" ht="14.25" customHeight="1">
       <c r="G977" s="3"/>
     </row>
-    <row r="978" ht="14.25" customHeight="1">
+    <row r="978" spans="7:7" ht="14.25" customHeight="1">
       <c r="G978" s="3"/>
     </row>
-    <row r="979" ht="14.25" customHeight="1">
+    <row r="979" spans="7:7" ht="14.25" customHeight="1">
       <c r="G979" s="3"/>
     </row>
-    <row r="980" ht="14.25" customHeight="1">
+    <row r="980" spans="7:7" ht="14.25" customHeight="1">
       <c r="G980" s="3"/>
     </row>
-    <row r="981" ht="14.25" customHeight="1">
+    <row r="981" spans="7:7" ht="14.25" customHeight="1">
       <c r="G981" s="3"/>
     </row>
-    <row r="982" ht="14.25" customHeight="1">
+    <row r="982" spans="7:7" ht="14.25" customHeight="1">
       <c r="G982" s="3"/>
     </row>
-    <row r="983" ht="14.25" customHeight="1">
+    <row r="983" spans="7:7" ht="14.25" customHeight="1">
       <c r="G983" s="3"/>
     </row>
-    <row r="984" ht="14.25" customHeight="1">
+    <row r="984" spans="7:7" ht="14.25" customHeight="1">
       <c r="G984" s="3"/>
     </row>
-    <row r="985" ht="14.25" customHeight="1">
+    <row r="985" spans="7:7" ht="14.25" customHeight="1">
       <c r="G985" s="3"/>
     </row>
-    <row r="986" ht="14.25" customHeight="1">
+    <row r="986" spans="7:7" ht="14.25" customHeight="1">
       <c r="G986" s="3"/>
     </row>
-    <row r="987" ht="14.25" customHeight="1">
+    <row r="987" spans="7:7" ht="14.25" customHeight="1">
       <c r="G987" s="3"/>
     </row>
-    <row r="988" ht="14.25" customHeight="1">
+    <row r="988" spans="7:7" ht="14.25" customHeight="1">
       <c r="G988" s="3"/>
     </row>
-    <row r="989" ht="14.25" customHeight="1">
+    <row r="989" spans="7:7" ht="14.25" customHeight="1">
       <c r="G989" s="3"/>
     </row>
-    <row r="990" ht="14.25" customHeight="1">
+    <row r="990" spans="7:7" ht="14.25" customHeight="1">
       <c r="G990" s="3"/>
     </row>
-    <row r="991" ht="14.25" customHeight="1">
+    <row r="991" spans="7:7" ht="14.25" customHeight="1">
       <c r="G991" s="3"/>
     </row>
-    <row r="992" ht="14.25" customHeight="1">
+    <row r="992" spans="7:7" ht="14.25" customHeight="1">
       <c r="G992" s="3"/>
     </row>
-    <row r="993" ht="14.25" customHeight="1">
+    <row r="993" spans="7:7" ht="14.25" customHeight="1">
       <c r="G993" s="3"/>
     </row>
-    <row r="994" ht="14.25" customHeight="1">
+    <row r="994" spans="7:7" ht="14.25" customHeight="1">
       <c r="G994" s="3"/>
     </row>
-    <row r="995" ht="14.25" customHeight="1">
+    <row r="995" spans="7:7" ht="14.25" customHeight="1">
       <c r="G995" s="3"/>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>